<commit_message>
belum berhasil membuat login
</commit_message>
<xml_diff>
--- a/backend/db_peg.xlsx
+++ b/backend/db_peg.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\awalokana_penilai_pemeriksa\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0965296-C606-4CB3-A086-A97715D14B0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFA33E31-BF56-4E8E-B304-1051549F54DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="601" activeTab="2" xr2:uid="{BC189E2B-F187-43D9-9614-18704A6CB784}"/>
   </bookViews>
@@ -7416,7 +7416,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="6" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -7527,24 +7527,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="13" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="6" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -36643,8 +36625,8 @@
   </sheetPr>
   <dimension ref="A1:X301"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="A289" zoomScale="145" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B312" sqref="B312"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="A274" zoomScale="145" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E285" sqref="E285"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37117,7 +37099,7 @@
         <v>1100</v>
       </c>
       <c r="L7" s="8"/>
-      <c r="M7" s="41"/>
+      <c r="M7" s="22"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
       <c r="P7" s="8" t="s">
@@ -37247,7 +37229,7 @@
         <v>1100</v>
       </c>
       <c r="L9" s="8"/>
-      <c r="M9" s="41"/>
+      <c r="M9" s="22"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
       <c r="P9" s="8" t="s">
@@ -37771,7 +37753,7 @@
         <v>1100</v>
       </c>
       <c r="L17" s="8"/>
-      <c r="M17" s="41"/>
+      <c r="M17" s="22"/>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
       <c r="P17" s="8" t="s">
@@ -37903,7 +37885,7 @@
         <v>1100</v>
       </c>
       <c r="L19" s="8"/>
-      <c r="M19" s="41"/>
+      <c r="M19" s="22"/>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
       <c r="P19" s="8" t="s">
@@ -38441,7 +38423,7 @@
         <v>1100</v>
       </c>
       <c r="L27" s="8"/>
-      <c r="M27" s="41"/>
+      <c r="M27" s="22"/>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
       <c r="P27" s="8" t="s">
@@ -38458,7 +38440,7 @@
       <c r="T27" s="13" t="s">
         <v>1528</v>
       </c>
-      <c r="U27" s="40"/>
+      <c r="U27" s="18"/>
       <c r="V27" s="14" t="str">
         <f>peg_nama2[[#This Row],[tmplahir]]&amp;", "&amp;TEXT(peg_nama2[[#This Row],[tgllahir]],"d MMM yyyy")</f>
         <v>Tapanuli Utara, 17 Mar 1968</v>
@@ -38705,7 +38687,7 @@
         <v>1100</v>
       </c>
       <c r="L31" s="8"/>
-      <c r="M31" s="41"/>
+      <c r="M31" s="22"/>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
       <c r="P31" s="8" t="s">
@@ -39141,7 +39123,7 @@
         <v>1100</v>
       </c>
       <c r="L37" s="8"/>
-      <c r="M37" s="41"/>
+      <c r="M37" s="22"/>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
       <c r="P37" s="8" t="s">
@@ -39207,7 +39189,7 @@
         <v>1100</v>
       </c>
       <c r="L38" s="8"/>
-      <c r="M38" s="41"/>
+      <c r="M38" s="22"/>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
       <c r="P38" s="8" t="s">
@@ -39275,7 +39257,7 @@
       <c r="L39" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="M39" s="42" t="s">
+      <c r="M39" s="16" t="s">
         <v>169</v>
       </c>
       <c r="N39" s="2"/>
@@ -39351,7 +39333,7 @@
       <c r="L40" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="M40" s="42" t="s">
+      <c r="M40" s="16" t="s">
         <v>150</v>
       </c>
       <c r="N40" s="2"/>
@@ -39500,8 +39482,8 @@
       <c r="K42" s="9" t="s">
         <v>1100</v>
       </c>
-      <c r="L42" s="41"/>
-      <c r="M42" s="41"/>
+      <c r="L42" s="22"/>
+      <c r="M42" s="22"/>
       <c r="N42" s="2"/>
       <c r="O42" s="2"/>
       <c r="P42" s="8" t="s">
@@ -39851,7 +39833,7 @@
         <v>1100</v>
       </c>
       <c r="L47" s="8"/>
-      <c r="M47" s="41"/>
+      <c r="M47" s="22"/>
       <c r="N47" s="2"/>
       <c r="O47" s="2"/>
       <c r="P47" s="8" t="s">
@@ -40071,7 +40053,7 @@
       <c r="L50" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="M50" s="42" t="s">
+      <c r="M50" s="16" t="s">
         <v>158</v>
       </c>
       <c r="N50" s="2"/>
@@ -40145,7 +40127,7 @@
         <v>1100</v>
       </c>
       <c r="L51" s="8"/>
-      <c r="M51" s="41"/>
+      <c r="M51" s="22"/>
       <c r="N51" s="2"/>
       <c r="O51" s="2"/>
       <c r="P51" s="8" t="s">
@@ -40933,7 +40915,7 @@
         <v>1100</v>
       </c>
       <c r="L62" s="8"/>
-      <c r="M62" s="41"/>
+      <c r="M62" s="22"/>
       <c r="N62" s="2"/>
       <c r="O62" s="2"/>
       <c r="P62" s="8" t="s">
@@ -41481,7 +41463,7 @@
         <v>1100</v>
       </c>
       <c r="L70" s="8"/>
-      <c r="M70" s="41"/>
+      <c r="M70" s="22"/>
       <c r="N70" s="2"/>
       <c r="O70" s="2"/>
       <c r="P70" s="8" t="s">
@@ -41959,7 +41941,7 @@
         <v>1100</v>
       </c>
       <c r="L77" s="8"/>
-      <c r="M77" s="41"/>
+      <c r="M77" s="22"/>
       <c r="N77" s="2"/>
       <c r="O77" s="2"/>
       <c r="P77" s="8" t="s">
@@ -42103,7 +42085,7 @@
         <v>1100</v>
       </c>
       <c r="L79" s="8"/>
-      <c r="M79" s="41"/>
+      <c r="M79" s="22"/>
       <c r="N79" s="2"/>
       <c r="O79" s="2"/>
       <c r="P79" s="8" t="s">
@@ -42168,8 +42150,8 @@
       <c r="K80" s="9" t="s">
         <v>1100</v>
       </c>
-      <c r="L80" s="41"/>
-      <c r="M80" s="41"/>
+      <c r="L80" s="22"/>
+      <c r="M80" s="22"/>
       <c r="N80" s="2"/>
       <c r="O80" s="2"/>
       <c r="P80" s="8" t="s">
@@ -42646,8 +42628,8 @@
       <c r="K87" s="9" t="s">
         <v>1100</v>
       </c>
-      <c r="L87" s="41"/>
-      <c r="M87" s="41"/>
+      <c r="L87" s="22"/>
+      <c r="M87" s="22"/>
       <c r="N87" s="2"/>
       <c r="O87" s="2"/>
       <c r="P87" s="8" t="s">
@@ -43042,8 +43024,8 @@
       <c r="K93" s="9" t="s">
         <v>1100</v>
       </c>
-      <c r="L93" s="41"/>
-      <c r="M93" s="41"/>
+      <c r="L93" s="22"/>
+      <c r="M93" s="22"/>
       <c r="N93" s="2"/>
       <c r="O93" s="2"/>
       <c r="P93" s="8" t="s">
@@ -43174,10 +43156,10 @@
       <c r="K95" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="L95" s="42" t="s">
+      <c r="L95" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="M95" s="42" t="s">
+      <c r="M95" s="16" t="s">
         <v>189</v>
       </c>
       <c r="N95" s="2"/>
@@ -43314,8 +43296,8 @@
       <c r="K97" s="9" t="s">
         <v>1100</v>
       </c>
-      <c r="L97" s="41"/>
-      <c r="M97" s="41"/>
+      <c r="L97" s="22"/>
+      <c r="M97" s="22"/>
       <c r="N97" s="2"/>
       <c r="O97" s="2"/>
       <c r="P97" s="8" t="s">
@@ -43380,8 +43362,8 @@
       <c r="K98" s="9" t="s">
         <v>1100</v>
       </c>
-      <c r="L98" s="41"/>
-      <c r="M98" s="41"/>
+      <c r="L98" s="22"/>
+      <c r="M98" s="22"/>
       <c r="N98" s="2"/>
       <c r="O98" s="2"/>
       <c r="P98" s="8" t="s">
@@ -43840,8 +43822,8 @@
       <c r="K105" s="9" t="s">
         <v>1100</v>
       </c>
-      <c r="L105" s="41"/>
-      <c r="M105" s="41"/>
+      <c r="L105" s="22"/>
+      <c r="M105" s="22"/>
       <c r="N105" s="2"/>
       <c r="O105" s="2"/>
       <c r="P105" s="8" t="s">
@@ -43906,10 +43888,10 @@
       <c r="K106" s="9" t="s">
         <v>283</v>
       </c>
-      <c r="L106" s="42" t="s">
+      <c r="L106" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="M106" s="42" t="s">
+      <c r="M106" s="16" t="s">
         <v>150</v>
       </c>
       <c r="N106" s="2"/>
@@ -43982,8 +43964,8 @@
       <c r="K107" s="9" t="s">
         <v>1100</v>
       </c>
-      <c r="L107" s="41"/>
-      <c r="M107" s="41"/>
+      <c r="L107" s="22"/>
+      <c r="M107" s="22"/>
       <c r="N107" s="2"/>
       <c r="O107" s="2"/>
       <c r="P107" s="8" t="s">
@@ -44124,8 +44106,8 @@
       <c r="K109" s="9" t="s">
         <v>1100</v>
       </c>
-      <c r="L109" s="41"/>
-      <c r="M109" s="41"/>
+      <c r="L109" s="22"/>
+      <c r="M109" s="22"/>
       <c r="N109" s="2"/>
       <c r="O109" s="2"/>
       <c r="P109" s="8" t="s">
@@ -44190,7 +44172,7 @@
       <c r="K110" s="9" t="s">
         <v>283</v>
       </c>
-      <c r="L110" s="42" t="s">
+      <c r="L110" s="16" t="s">
         <v>149</v>
       </c>
       <c r="M110" s="16" t="s">
@@ -44664,8 +44646,8 @@
       <c r="K117" s="9" t="s">
         <v>1100</v>
       </c>
-      <c r="L117" s="41"/>
-      <c r="M117" s="41"/>
+      <c r="L117" s="22"/>
+      <c r="M117" s="22"/>
       <c r="N117" s="2"/>
       <c r="O117" s="2"/>
       <c r="P117" s="8" t="s">
@@ -44796,8 +44778,8 @@
       <c r="K119" s="9" t="s">
         <v>1100</v>
       </c>
-      <c r="L119" s="41"/>
-      <c r="M119" s="41"/>
+      <c r="L119" s="22"/>
+      <c r="M119" s="22"/>
       <c r="N119" s="2"/>
       <c r="O119" s="2"/>
       <c r="P119" s="8" t="s">
@@ -45422,8 +45404,8 @@
       <c r="K128" s="9" t="s">
         <v>1100</v>
       </c>
-      <c r="L128" s="41"/>
-      <c r="M128" s="41"/>
+      <c r="L128" s="22"/>
+      <c r="M128" s="22"/>
       <c r="N128" s="2"/>
       <c r="O128" s="2"/>
       <c r="P128" s="8" t="s">
@@ -45488,8 +45470,8 @@
       <c r="K129" s="9" t="s">
         <v>1100</v>
       </c>
-      <c r="L129" s="41"/>
-      <c r="M129" s="41"/>
+      <c r="L129" s="22"/>
+      <c r="M129" s="22"/>
       <c r="N129" s="2"/>
       <c r="O129" s="2"/>
       <c r="P129" s="8" t="s">
@@ -45554,8 +45536,8 @@
       <c r="K130" s="9" t="s">
         <v>1100</v>
       </c>
-      <c r="L130" s="41"/>
-      <c r="M130" s="41"/>
+      <c r="L130" s="22"/>
+      <c r="M130" s="22"/>
       <c r="N130" s="2"/>
       <c r="O130" s="2"/>
       <c r="P130" s="8" t="s">
@@ -46067,7 +46049,7 @@
         <v>1100</v>
       </c>
       <c r="L137" s="8"/>
-      <c r="M137" s="41"/>
+      <c r="M137" s="22"/>
       <c r="N137" s="2"/>
       <c r="O137" s="2"/>
       <c r="P137" s="8" t="s">
@@ -46274,10 +46256,10 @@
       <c r="K140" s="9" t="s">
         <v>945</v>
       </c>
-      <c r="L140" s="42" t="s">
+      <c r="L140" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="M140" s="42" t="s">
+      <c r="M140" s="16" t="s">
         <v>199</v>
       </c>
       <c r="N140" s="2"/>
@@ -46898,8 +46880,8 @@
       <c r="K149" s="9" t="s">
         <v>1100</v>
       </c>
-      <c r="L149" s="41"/>
-      <c r="M149" s="41"/>
+      <c r="L149" s="22"/>
+      <c r="M149" s="22"/>
       <c r="N149" s="2"/>
       <c r="O149" s="2"/>
       <c r="P149" s="8" t="s">
@@ -47172,8 +47154,8 @@
       <c r="K153" s="9" t="s">
         <v>1100</v>
       </c>
-      <c r="L153" s="41"/>
-      <c r="M153" s="41"/>
+      <c r="L153" s="22"/>
+      <c r="M153" s="22"/>
       <c r="N153" s="2"/>
       <c r="O153" s="2"/>
       <c r="P153" s="8" t="s">
@@ -47766,7 +47748,7 @@
       <c r="T161" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="U161" s="40">
+      <c r="U161" s="18">
         <v>42361</v>
       </c>
       <c r="V161" s="14" t="str">
@@ -47958,10 +47940,10 @@
       <c r="K164" s="9" t="s">
         <v>283</v>
       </c>
-      <c r="L164" s="42" t="s">
+      <c r="L164" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="M164" s="42" t="s">
+      <c r="M164" s="16" t="s">
         <v>158</v>
       </c>
       <c r="N164" s="2"/>
@@ -48166,8 +48148,8 @@
       <c r="K167" s="9" t="s">
         <v>1100</v>
       </c>
-      <c r="L167" s="41"/>
-      <c r="M167" s="41"/>
+      <c r="L167" s="22"/>
+      <c r="M167" s="22"/>
       <c r="N167" s="2"/>
       <c r="O167" s="2"/>
       <c r="P167" s="8" t="s">
@@ -48374,10 +48356,10 @@
       <c r="K170" s="9" t="s">
         <v>283</v>
       </c>
-      <c r="L170" s="42" t="s">
+      <c r="L170" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="M170" s="42" t="s">
+      <c r="M170" s="16" t="s">
         <v>158</v>
       </c>
       <c r="N170" s="2"/>
@@ -48516,8 +48498,8 @@
       <c r="K172" s="9" t="s">
         <v>1100</v>
       </c>
-      <c r="L172" s="41"/>
-      <c r="M172" s="41"/>
+      <c r="L172" s="22"/>
+      <c r="M172" s="22"/>
       <c r="N172" s="2"/>
       <c r="O172" s="2"/>
       <c r="P172" s="8" t="s">
@@ -48798,10 +48780,10 @@
       <c r="K176" s="9" t="s">
         <v>1099</v>
       </c>
-      <c r="L176" s="42" t="s">
+      <c r="L176" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="M176" s="42" t="s">
+      <c r="M176" s="16" t="s">
         <v>199</v>
       </c>
       <c r="N176" s="2"/>
@@ -48938,8 +48920,8 @@
       <c r="K178" s="9" t="s">
         <v>1100</v>
       </c>
-      <c r="L178" s="41"/>
-      <c r="M178" s="41"/>
+      <c r="L178" s="22"/>
+      <c r="M178" s="22"/>
       <c r="N178" s="2"/>
       <c r="O178" s="2"/>
       <c r="P178" s="8" t="s">
@@ -49022,7 +49004,7 @@
       <c r="T179" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="U179" s="40"/>
+      <c r="U179" s="18"/>
       <c r="V179" s="14" t="str">
         <f>peg_nama2[[#This Row],[tmplahir]]&amp;", "&amp;TEXT(peg_nama2[[#This Row],[tgllahir]],"d MMM yyyy")</f>
         <v>Pangkal Pinang, 6 Jan 1987</v>
@@ -49428,8 +49410,8 @@
       <c r="K185" s="9" t="s">
         <v>1100</v>
       </c>
-      <c r="L185" s="41"/>
-      <c r="M185" s="41"/>
+      <c r="L185" s="22"/>
+      <c r="M185" s="22"/>
       <c r="N185" s="2"/>
       <c r="O185" s="2"/>
       <c r="P185" s="8" t="s">
@@ -49584,7 +49566,7 @@
         <v>1014</v>
       </c>
       <c r="T187" s="13"/>
-      <c r="U187" s="40">
+      <c r="U187" s="18">
         <v>39965</v>
       </c>
       <c r="V187" s="14" t="str">
@@ -49700,8 +49682,8 @@
       <c r="K189" s="9" t="s">
         <v>1100</v>
       </c>
-      <c r="L189" s="41"/>
-      <c r="M189" s="41"/>
+      <c r="L189" s="22"/>
+      <c r="M189" s="22"/>
       <c r="N189" s="2"/>
       <c r="O189" s="2"/>
       <c r="P189" s="8" t="s">
@@ -49718,7 +49700,7 @@
       <c r="T189" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="U189" s="40"/>
+      <c r="U189" s="18"/>
       <c r="V189" s="14" t="str">
         <f>peg_nama2[[#This Row],[tmplahir]]&amp;", "&amp;TEXT(peg_nama2[[#This Row],[tgllahir]],"d MMM yyyy")</f>
         <v>Denpasar, 14 Jan 1983</v>
@@ -49832,10 +49814,10 @@
       <c r="K191" s="9" t="s">
         <v>1028</v>
       </c>
-      <c r="L191" s="42" t="s">
+      <c r="L191" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="M191" s="42" t="s">
+      <c r="M191" s="16" t="s">
         <v>169</v>
       </c>
       <c r="N191" s="2"/>
@@ -50040,8 +50022,8 @@
       <c r="K194" s="9" t="s">
         <v>1100</v>
       </c>
-      <c r="L194" s="41"/>
-      <c r="M194" s="41"/>
+      <c r="L194" s="22"/>
+      <c r="M194" s="22"/>
       <c r="N194" s="2"/>
       <c r="O194" s="2"/>
       <c r="P194" s="8" t="s">
@@ -50454,8 +50436,8 @@
       <c r="K200" s="9" t="s">
         <v>1100</v>
       </c>
-      <c r="L200" s="41"/>
-      <c r="M200" s="41"/>
+      <c r="L200" s="22"/>
+      <c r="M200" s="22"/>
       <c r="N200" s="2"/>
       <c r="O200" s="2"/>
       <c r="P200" s="8" t="s">
@@ -51364,7 +51346,7 @@
       <c r="K213" s="9" t="s">
         <v>996</v>
       </c>
-      <c r="L213" s="42" t="s">
+      <c r="L213" s="16" t="s">
         <v>136</v>
       </c>
       <c r="M213" s="16" t="s">
@@ -51925,8 +51907,8 @@
       <c r="K221" s="9" t="s">
         <v>1100</v>
       </c>
-      <c r="L221" s="41"/>
-      <c r="M221" s="41"/>
+      <c r="L221" s="22"/>
+      <c r="M221" s="22"/>
       <c r="N221" s="2"/>
       <c r="O221" s="2"/>
       <c r="P221" s="8" t="s">
@@ -52057,10 +52039,10 @@
       <c r="K223" s="9" t="s">
         <v>435</v>
       </c>
-      <c r="L223" s="42" t="s">
+      <c r="L223" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="M223" s="42" t="s">
+      <c r="M223" s="16" t="s">
         <v>158</v>
       </c>
       <c r="N223" s="2"/>
@@ -52199,8 +52181,8 @@
       <c r="K225" s="9" t="s">
         <v>1100</v>
       </c>
-      <c r="L225" s="41"/>
-      <c r="M225" s="41"/>
+      <c r="L225" s="22"/>
+      <c r="M225" s="22"/>
       <c r="N225" s="2"/>
       <c r="O225" s="2"/>
       <c r="P225" s="8" t="s">
@@ -52407,8 +52389,8 @@
       <c r="K228" s="9" t="s">
         <v>1100</v>
       </c>
-      <c r="L228" s="41"/>
-      <c r="M228" s="41"/>
+      <c r="L228" s="22"/>
+      <c r="M228" s="22"/>
       <c r="N228" s="2"/>
       <c r="O228" s="2"/>
       <c r="P228" s="8" t="s">
@@ -53181,10 +53163,10 @@
       <c r="K239" s="9" t="s">
         <v>435</v>
       </c>
-      <c r="L239" s="42" t="s">
+      <c r="L239" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="M239" s="42" t="s">
+      <c r="M239" s="16" t="s">
         <v>158</v>
       </c>
       <c r="N239" s="2"/>
@@ -53207,7 +53189,7 @@
       <c r="T239" s="13" t="s">
         <v>566</v>
       </c>
-      <c r="U239" s="40">
+      <c r="U239" s="18">
         <v>43525</v>
       </c>
       <c r="V239" s="14" t="str">
@@ -53789,10 +53771,10 @@
       <c r="K247" s="9" t="s">
         <v>1028</v>
       </c>
-      <c r="L247" s="42" t="s">
+      <c r="L247" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="M247" s="42" t="s">
+      <c r="M247" s="16" t="s">
         <v>189</v>
       </c>
       <c r="N247" s="2"/>
@@ -54698,7 +54680,7 @@
       <c r="L259" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="M259" s="42" t="s">
+      <c r="M259" s="16" t="s">
         <v>207</v>
       </c>
       <c r="N259" s="2"/>
@@ -54845,10 +54827,10 @@
       <c r="K261" s="9" t="s">
         <v>435</v>
       </c>
-      <c r="L261" s="42" t="s">
+      <c r="L261" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="M261" s="42" t="s">
+      <c r="M261" s="16" t="s">
         <v>158</v>
       </c>
       <c r="N261" s="2"/>
@@ -55453,10 +55435,10 @@
       <c r="K269" s="9" t="s">
         <v>435</v>
       </c>
-      <c r="L269" s="42" t="s">
+      <c r="L269" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="M269" s="42" t="s">
+      <c r="M269" s="16" t="s">
         <v>150</v>
       </c>
       <c r="N269" s="2"/>
@@ -56061,10 +56043,10 @@
       <c r="K277" s="9" t="s">
         <v>435</v>
       </c>
-      <c r="L277" s="42" t="s">
+      <c r="L277" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="M277" s="42" t="s">
+      <c r="M277" s="16" t="s">
         <v>150</v>
       </c>
       <c r="N277" s="2"/>
@@ -56265,7 +56247,7 @@
       <c r="C280" s="2" t="s">
         <v>670</v>
       </c>
-      <c r="D280" s="2" t="s">
+      <c r="D280" s="20" t="s">
         <v>671</v>
       </c>
       <c r="E280" s="2" t="s">
@@ -56365,10 +56347,10 @@
       <c r="K281" s="9" t="s">
         <v>435</v>
       </c>
-      <c r="L281" s="42" t="s">
+      <c r="L281" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="M281" s="42" t="s">
+      <c r="M281" s="16" t="s">
         <v>158</v>
       </c>
       <c r="N281" s="2"/>
@@ -56441,10 +56423,10 @@
       <c r="K282" s="9" t="s">
         <v>435</v>
       </c>
-      <c r="L282" s="42" t="s">
+      <c r="L282" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="M282" s="42" t="s">
+      <c r="M282" s="16" t="s">
         <v>158</v>
       </c>
       <c r="N282" s="2"/>
@@ -56593,10 +56575,10 @@
       <c r="K284" s="9" t="s">
         <v>435</v>
       </c>
-      <c r="L284" s="42" t="s">
+      <c r="L284" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="M284" s="42" t="s">
+      <c r="M284" s="16" t="s">
         <v>158</v>
       </c>
       <c r="N284" s="2"/>
@@ -56949,7 +56931,7 @@
       <c r="C289" s="2" t="s">
         <v>761</v>
       </c>
-      <c r="D289" s="2" t="s">
+      <c r="D289" s="20" t="s">
         <v>762</v>
       </c>
       <c r="E289" s="2" t="s">
@@ -56973,10 +56955,10 @@
       <c r="K289" s="9" t="s">
         <v>435</v>
       </c>
-      <c r="L289" s="42" t="s">
+      <c r="L289" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="M289" s="42" t="s">
+      <c r="M289" s="16" t="s">
         <v>150</v>
       </c>
       <c r="N289" s="2"/>
@@ -57455,7 +57437,7 @@
       <c r="T295" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="U295" s="40">
+      <c r="U295" s="18">
         <v>44621</v>
       </c>
       <c r="V295" s="14" t="str">
@@ -57505,10 +57487,10 @@
       <c r="K296" s="9" t="s">
         <v>435</v>
       </c>
-      <c r="L296" s="42" t="s">
+      <c r="L296" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="M296" s="42" t="s">
+      <c r="M296" s="16" t="s">
         <v>150</v>
       </c>
       <c r="N296" s="2"/>
@@ -57798,8 +57780,8 @@
       <c r="K300" s="9" t="s">
         <v>1100</v>
       </c>
-      <c r="L300" s="41"/>
-      <c r="M300" s="41"/>
+      <c r="L300" s="22"/>
+      <c r="M300" s="22"/>
       <c r="N300" s="3"/>
       <c r="O300" s="3"/>
       <c r="P300" s="27" t="s">
@@ -57831,31 +57813,31 @@
       </c>
     </row>
     <row r="301" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A301" s="38" t="s">
+      <c r="A301" s="30" t="s">
         <v>428</v>
       </c>
-      <c r="B301" s="39" t="s">
+      <c r="B301" s="31" t="s">
         <v>429</v>
       </c>
-      <c r="C301" s="39" t="s">
+      <c r="C301" s="31" t="s">
         <v>430</v>
       </c>
-      <c r="D301" s="39" t="s">
+      <c r="D301" s="31" t="s">
         <v>431</v>
       </c>
-      <c r="E301" s="39" t="s">
+      <c r="E301" s="31" t="s">
         <v>432</v>
       </c>
-      <c r="F301" s="40">
+      <c r="F301" s="18">
         <v>28185</v>
       </c>
-      <c r="G301" s="39" t="s">
+      <c r="G301" s="31" t="s">
         <v>433</v>
       </c>
-      <c r="H301" s="39" t="s">
+      <c r="H301" s="31" t="s">
         <v>434</v>
       </c>
-      <c r="I301" s="41">
+      <c r="I301" s="22">
         <v>2008</v>
       </c>
       <c r="J301" s="9" t="s">
@@ -57870,27 +57852,27 @@
       <c r="M301" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="N301" s="39"/>
-      <c r="O301" s="39" t="s">
+      <c r="N301" s="31"/>
+      <c r="O301" s="31" t="s">
         <v>436</v>
       </c>
-      <c r="P301" s="41" t="s">
-        <v>123</v>
-      </c>
-      <c r="Q301" s="41" t="s">
+      <c r="P301" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q301" s="22" t="s">
         <v>124</v>
       </c>
       <c r="R301" s="32" t="str">
         <f>IF(MID(peg_nama2[[#This Row],[nip]],15,1)="1","Laki-laki","Perempuan")</f>
         <v>Laki-laki</v>
       </c>
-      <c r="S301" s="38" t="s">
+      <c r="S301" s="30" t="s">
         <v>437</v>
       </c>
-      <c r="T301" s="43" t="s">
+      <c r="T301" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="U301" s="40">
+      <c r="U301" s="18">
         <v>44529</v>
       </c>
       <c r="V301" s="14" t="str">
@@ -57934,11 +57916,13 @@
     <hyperlink ref="G4" r:id="rId24" xr:uid="{2321C8FC-A150-480F-B971-C88C8703D2E9}"/>
     <hyperlink ref="H300" r:id="rId25" xr:uid="{9AF3C8A2-AD6E-4C3A-9F19-3E273F675899}"/>
     <hyperlink ref="H4" r:id="rId26" xr:uid="{044BE42A-F4F0-4732-943F-F3ACD9380C5D}"/>
+    <hyperlink ref="D289" r:id="rId27" xr:uid="{CBE8B68F-B5D2-40A7-A294-95D9B5E685AD}"/>
+    <hyperlink ref="D280" r:id="rId28" xr:uid="{6B30C7C8-69D2-4831-B921-AA49E25E4EB2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId27"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId29"/>
   <tableParts count="1">
-    <tablePart r:id="rId28"/>
+    <tablePart r:id="rId30"/>
   </tableParts>
 </worksheet>
 </file>
@@ -57953,17 +57937,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="35e2c585-819f-4278-8a16-df2610a1755b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="a5904320-7c22-4772-b594-ceafc042e3d2" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FF8157A31B2A7C4BB85FD3832F8712B1" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d18c389983c6f9b98ad163ecd6856692">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="35e2c585-819f-4278-8a16-df2610a1755b" xmlns:ns3="a5904320-7c22-4772-b594-ceafc042e3d2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ac16c791c24eb0f84a04be040c4dde29" ns2:_="" ns3:_="">
     <xsd:import namespace="35e2c585-819f-4278-8a16-df2610a1755b"/>
@@ -58158,6 +58131,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="35e2c585-819f-4278-8a16-df2610a1755b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="a5904320-7c22-4772-b594-ceafc042e3d2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{623689F7-DDC4-43DC-AB5C-EAB680CA80A6}">
   <ds:schemaRefs>
@@ -58167,17 +58151,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5018FBA8-FFB9-4942-93FE-3D9DBCE7EB9C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="35e2c585-819f-4278-8a16-df2610a1755b"/>
-    <ds:schemaRef ds:uri="a5904320-7c22-4772-b594-ceafc042e3d2"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E88B49FB-5345-49B6-AE64-3BD78824E406}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -58194,4 +58167,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5018FBA8-FFB9-4942-93FE-3D9DBCE7EB9C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="35e2c585-819f-4278-8a16-df2610a1755b"/>
+    <ds:schemaRef ds:uri="a5904320-7c22-4772-b594-ceafc042e3d2"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
kurang sistem voting dan penilaian kinerja
</commit_message>
<xml_diff>
--- a/backend/db_peg.xlsx
+++ b/backend/db_peg.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\awalokana_penilai_pemeriksa\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFA33E31-BF56-4E8E-B304-1051549F54DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC8717C-B2C1-47AB-B615-B3B54409095F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="601" activeTab="2" xr2:uid="{BC189E2B-F187-43D9-9614-18704A6CB784}"/>
   </bookViews>
@@ -7287,12 +7287,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -7416,7 +7417,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="6" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -7529,6 +7530,24 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="13" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="2" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="1" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="1" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="Comma [0] 2" xfId="7" xr:uid="{33A97758-E3EE-48C7-A301-AA64A4453F49}"/>
@@ -7548,6 +7567,42 @@
     <cellStyle name="Normal 3" xfId="5" xr:uid="{70B4B239-ED42-4381-8963-55714BE10C2B}"/>
   </cellStyles>
   <dxfs count="72">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd;@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -8056,42 +8111,6 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -9676,31 +9695,31 @@
     <tableColumn id="4" xr3:uid="{FE3C082E-EF4A-4D3E-B2D1-193C49FCA0CB}" name="nip" dataDxfId="21"/>
     <tableColumn id="5" xr3:uid="{36F05CC3-D119-4189-8605-7EAC4A7DD705}" name="email" dataDxfId="20"/>
     <tableColumn id="6" xr3:uid="{A647F0D1-EAF4-4FDC-BE84-C4D08D64DFEE}" name="tmplahir" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{5A3B33E8-E47A-460F-827A-F4E657B6F7CC}" name="tgllahir" dataDxfId="18"/>
-    <tableColumn id="8" xr3:uid="{AE92D20C-F51D-41EF-AC1B-FCD77B9A082B}" name="profillink" dataDxfId="17"/>
-    <tableColumn id="9" xr3:uid="{14068D43-500B-4201-AF1F-CB0C19346DC6}" name="fotolink" dataDxfId="16"/>
-    <tableColumn id="10" xr3:uid="{08257D47-DE3F-4606-BE20-D1FBCBE79847}" name="angkatan" dataDxfId="15"/>
-    <tableColumn id="21" xr3:uid="{A8D85F63-3E20-4627-AC0E-1B02FDFC3373}" name="jnsjab" dataDxfId="14" dataCellStyle="Normal 2 3"/>
-    <tableColumn id="25" xr3:uid="{DF226D36-7E4D-4921-960F-33595FBB5426}" name="jab" dataDxfId="13" dataCellStyle="Normal 2 3"/>
-    <tableColumn id="22" xr3:uid="{72C7675E-EC04-4646-9AB5-E48D973C12ED}" name="unker" dataDxfId="12" dataCellStyle="Normal 2 3"/>
-    <tableColumn id="13" xr3:uid="{6BBB15D6-D09E-4EE6-9460-42762BB61DCF}" name="subunker" dataDxfId="11"/>
-    <tableColumn id="14" xr3:uid="{7BDB0558-5D09-47B6-B15C-89BE6BD257B7}" name="titeldepan" dataDxfId="10"/>
-    <tableColumn id="15" xr3:uid="{FD2BA64B-2050-4B89-868B-E4E6B206C2BE}" name="titelbelakang" dataDxfId="9"/>
-    <tableColumn id="16" xr3:uid="{C1F3A17B-5F16-4AC5-8D51-338E104E02D8}" name="statpeg" dataDxfId="8"/>
-    <tableColumn id="17" xr3:uid="{788E3A38-BFCD-4205-BEA6-9C6000F032E8}" name="aktifpeg" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{C8586149-33A1-43BB-AF66-744EB307A328}" name="jnskel" dataDxfId="6">
+    <tableColumn id="7" xr3:uid="{5A3B33E8-E47A-460F-827A-F4E657B6F7CC}" name="tgllahir" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{AE92D20C-F51D-41EF-AC1B-FCD77B9A082B}" name="profillink" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{14068D43-500B-4201-AF1F-CB0C19346DC6}" name="fotolink" dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{08257D47-DE3F-4606-BE20-D1FBCBE79847}" name="angkatan" dataDxfId="16"/>
+    <tableColumn id="21" xr3:uid="{A8D85F63-3E20-4627-AC0E-1B02FDFC3373}" name="jnsjab" dataDxfId="15" dataCellStyle="Normal 2 3"/>
+    <tableColumn id="25" xr3:uid="{DF226D36-7E4D-4921-960F-33595FBB5426}" name="jab" dataDxfId="14" dataCellStyle="Normal 2 3"/>
+    <tableColumn id="22" xr3:uid="{72C7675E-EC04-4646-9AB5-E48D973C12ED}" name="unker" dataDxfId="13" dataCellStyle="Normal 2 3"/>
+    <tableColumn id="13" xr3:uid="{6BBB15D6-D09E-4EE6-9460-42762BB61DCF}" name="subunker" dataDxfId="12"/>
+    <tableColumn id="14" xr3:uid="{7BDB0558-5D09-47B6-B15C-89BE6BD257B7}" name="titeldepan" dataDxfId="11"/>
+    <tableColumn id="15" xr3:uid="{FD2BA64B-2050-4B89-868B-E4E6B206C2BE}" name="titelbelakang" dataDxfId="10"/>
+    <tableColumn id="16" xr3:uid="{C1F3A17B-5F16-4AC5-8D51-338E104E02D8}" name="statpeg" dataDxfId="9"/>
+    <tableColumn id="17" xr3:uid="{788E3A38-BFCD-4205-BEA6-9C6000F032E8}" name="aktifpeg" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{C8586149-33A1-43BB-AF66-744EB307A328}" name="jnskel" dataDxfId="7">
       <calculatedColumnFormula>IF(MID(peg_nama2[[#This Row],[nip]],15,1)="1","Laki-laki","Perempuan")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{C0EF9A4E-A2CB-49DF-B6D1-9516F75B0CDD}" name="ponsel" dataDxfId="5"/>
-    <tableColumn id="12" xr3:uid="{9815D0AF-0FD0-4CF7-85DC-3B29F7E4ABF5}" name="latdik" dataDxfId="4"/>
-    <tableColumn id="18" xr3:uid="{7C86715B-1BBD-4512-929B-9E8AC3FB13B2}" name="tmtbali" dataDxfId="3"/>
-    <tableColumn id="20" xr3:uid="{8DDCD0F6-22B2-4A6C-9470-3928368733CC}" name="ttl" dataDxfId="2">
+    <tableColumn id="19" xr3:uid="{C0EF9A4E-A2CB-49DF-B6D1-9516F75B0CDD}" name="ponsel" dataDxfId="6"/>
+    <tableColumn id="12" xr3:uid="{9815D0AF-0FD0-4CF7-85DC-3B29F7E4ABF5}" name="latdik" dataDxfId="5"/>
+    <tableColumn id="18" xr3:uid="{7C86715B-1BBD-4512-929B-9E8AC3FB13B2}" name="tmtbali" dataDxfId="4"/>
+    <tableColumn id="20" xr3:uid="{8DDCD0F6-22B2-4A6C-9470-3928368733CC}" name="ttl" dataDxfId="3">
       <calculatedColumnFormula>peg_nama2[[#This Row],[tmplahir]]&amp;", "&amp;TEXT(peg_nama2[[#This Row],[tgllahir]],"d mmmm yyyy")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{21898EA7-C523-4C56-A4CF-89EC14934B98}" name="teamslink" dataDxfId="1">
+    <tableColumn id="23" xr3:uid="{21898EA7-C523-4C56-A4CF-89EC14934B98}" name="teamslink" dataDxfId="2">
       <calculatedColumnFormula>"https://teams.microsoft.com/l/chat/0/0?users="&amp;peg_nama2[[#This Row],[email]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{4028D7C0-75D9-460F-8C9E-A756865B34E9}" name="walink" dataDxfId="0">
+    <tableColumn id="24" xr3:uid="{4028D7C0-75D9-460F-8C9E-A756865B34E9}" name="walink" dataDxfId="1">
       <calculatedColumnFormula>"https://wa.me/"&amp;peg_nama2[[#This Row],[ponsel]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -36625,8 +36644,8 @@
   </sheetPr>
   <dimension ref="A1:X301"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="A274" zoomScale="145" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E285" sqref="E285"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="E1" zoomScale="145" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36636,7 +36655,7 @@
     <col min="3" max="3" width="20.42578125" style="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.28515625" style="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.28515625" style="16" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" style="43" customWidth="1"/>
     <col min="7" max="7" width="60.28515625" style="16" customWidth="1"/>
     <col min="8" max="8" width="41.28515625" style="16" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" style="16" customWidth="1"/>
@@ -36674,7 +36693,7 @@
       <c r="E1" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="38" t="s">
         <v>95</v>
       </c>
       <c r="G1" s="4" t="s">
@@ -36748,7 +36767,7 @@
       <c r="E2" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="39">
         <v>23287</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -36812,7 +36831,7 @@
       <c r="E3" s="2" t="s">
         <v>886</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="39">
         <v>26231</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -36876,7 +36895,7 @@
       <c r="E4" s="2" t="s">
         <v>1252</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="39">
         <v>26561</v>
       </c>
       <c r="G4" s="21" t="s">
@@ -36952,7 +36971,7 @@
       <c r="E5" s="2" t="s">
         <v>1100</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="39">
         <v>20393</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -37016,7 +37035,7 @@
       <c r="E6" s="2" t="s">
         <v>1100</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="39">
         <v>20994</v>
       </c>
       <c r="G6" s="2" t="s">
@@ -37080,7 +37099,7 @@
       <c r="E7" s="2" t="s">
         <v>1381</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="39">
         <v>22497</v>
       </c>
       <c r="G7" s="2" t="s">
@@ -37146,7 +37165,7 @@
       <c r="E8" s="2" t="s">
         <v>1100</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="39">
         <v>20820</v>
       </c>
       <c r="G8" s="2" t="s">
@@ -37210,7 +37229,7 @@
       <c r="E9" s="2" t="s">
         <v>1100</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="39">
         <v>20980</v>
       </c>
       <c r="G9" s="2" t="s">
@@ -37274,7 +37293,7 @@
       <c r="E10" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="39">
         <v>23375</v>
       </c>
       <c r="G10" s="2" t="s">
@@ -37340,7 +37359,7 @@
       <c r="E11" s="2" t="s">
         <v>1406</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="39">
         <v>23212</v>
       </c>
       <c r="G11" s="2" t="s">
@@ -37406,7 +37425,7 @@
       <c r="E12" s="2" t="s">
         <v>1100</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="39">
         <v>20939</v>
       </c>
       <c r="G12" s="2" t="s">
@@ -37470,7 +37489,7 @@
       <c r="E13" s="2" t="s">
         <v>483</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="39">
         <v>22559</v>
       </c>
       <c r="G13" s="2" t="s">
@@ -37536,7 +37555,7 @@
       <c r="E14" s="2" t="s">
         <v>468</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="39">
         <v>21383</v>
       </c>
       <c r="G14" s="20" t="s">
@@ -37602,7 +37621,7 @@
       <c r="E15" s="2" t="s">
         <v>1100</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="39">
         <v>22437</v>
       </c>
       <c r="G15" s="2" t="s">
@@ -37668,7 +37687,7 @@
       <c r="E16" s="2" t="s">
         <v>1439</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="39">
         <v>25297</v>
       </c>
       <c r="G16" s="2" t="s">
@@ -37734,7 +37753,7 @@
       <c r="E17" s="2" t="s">
         <v>1446</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="39">
         <v>23059</v>
       </c>
       <c r="G17" s="2" t="s">
@@ -37800,7 +37819,7 @@
       <c r="E18" s="2" t="s">
         <v>1460</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="39">
         <v>25720</v>
       </c>
       <c r="G18" s="2" t="s">
@@ -37866,7 +37885,7 @@
       <c r="E19" s="2" t="s">
         <v>1453</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="39">
         <v>22696</v>
       </c>
       <c r="G19" s="2" t="s">
@@ -37932,7 +37951,7 @@
       <c r="E20" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="39">
         <v>24805</v>
       </c>
       <c r="G20" s="2" t="s">
@@ -38008,7 +38027,7 @@
       <c r="E21" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="39">
         <v>27556</v>
       </c>
       <c r="G21" s="2" t="s">
@@ -38074,7 +38093,7 @@
       <c r="E22" s="2" t="s">
         <v>468</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F22" s="39">
         <v>27612</v>
       </c>
       <c r="G22" s="2" t="s">
@@ -38140,7 +38159,7 @@
       <c r="E23" s="2" t="s">
         <v>1491</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="39">
         <v>27150</v>
       </c>
       <c r="G23" s="2" t="s">
@@ -38206,7 +38225,7 @@
       <c r="E24" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F24" s="39">
         <v>24282</v>
       </c>
       <c r="G24" s="2" t="s">
@@ -38272,7 +38291,7 @@
       <c r="E25" s="2" t="s">
         <v>1504</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F25" s="39">
         <v>27722</v>
       </c>
       <c r="G25" s="2" t="s">
@@ -38338,7 +38357,7 @@
       <c r="E26" s="2" t="s">
         <v>1533</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F26" s="39">
         <v>25874</v>
       </c>
       <c r="G26" s="2" t="s">
@@ -38404,7 +38423,7 @@
       <c r="E27" s="2" t="s">
         <v>1525</v>
       </c>
-      <c r="F27" s="7">
+      <c r="F27" s="39">
         <v>24914</v>
       </c>
       <c r="G27" s="2" t="s">
@@ -38470,7 +38489,7 @@
       <c r="E28" s="2" t="s">
         <v>1511</v>
       </c>
-      <c r="F28" s="7">
+      <c r="F28" s="39">
         <v>25183</v>
       </c>
       <c r="G28" s="2" t="s">
@@ -38536,7 +38555,7 @@
       <c r="E29" s="2" t="s">
         <v>1518</v>
       </c>
-      <c r="F29" s="7">
+      <c r="F29" s="39">
         <v>24921</v>
       </c>
       <c r="G29" s="2" t="s">
@@ -38602,7 +38621,7 @@
       <c r="E30" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="F30" s="7">
+      <c r="F30" s="39">
         <v>26677</v>
       </c>
       <c r="G30" s="2" t="s">
@@ -38668,7 +38687,7 @@
       <c r="E31" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="F31" s="7">
+      <c r="F31" s="39">
         <v>24836</v>
       </c>
       <c r="G31" s="2" t="s">
@@ -38734,7 +38753,7 @@
       <c r="E32" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="F32" s="7">
+      <c r="F32" s="39">
         <v>26312</v>
       </c>
       <c r="G32" s="2" t="s">
@@ -38810,7 +38829,7 @@
       <c r="E33" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F33" s="7">
+      <c r="F33" s="39">
         <v>26536</v>
       </c>
       <c r="G33" s="2" t="s">
@@ -38886,7 +38905,7 @@
       <c r="E34" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="F34" s="7">
+      <c r="F34" s="39">
         <v>26224</v>
       </c>
       <c r="G34" s="19" t="s">
@@ -38962,7 +38981,7 @@
       <c r="E35" s="2" t="s">
         <v>886</v>
       </c>
-      <c r="F35" s="7">
+      <c r="F35" s="39">
         <v>26177</v>
       </c>
       <c r="G35" s="2" t="s">
@@ -39028,7 +39047,7 @@
       <c r="E36" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F36" s="7">
+      <c r="F36" s="39">
         <v>26790</v>
       </c>
       <c r="G36" s="2" t="s">
@@ -39104,7 +39123,7 @@
       <c r="E37" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F37" s="7">
+      <c r="F37" s="39">
         <v>27210</v>
       </c>
       <c r="G37" s="2" t="s">
@@ -39170,7 +39189,7 @@
       <c r="E38" s="2" t="s">
         <v>1584</v>
       </c>
-      <c r="F38" s="7">
+      <c r="F38" s="39">
         <v>26061</v>
       </c>
       <c r="G38" s="2" t="s">
@@ -39236,7 +39255,7 @@
       <c r="E39" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F39" s="7">
+      <c r="F39" s="39">
         <v>25863</v>
       </c>
       <c r="G39" s="2" t="s">
@@ -39312,7 +39331,7 @@
       <c r="E40" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="F40" s="7">
+      <c r="F40" s="39">
         <v>26326</v>
       </c>
       <c r="G40" s="2" t="s">
@@ -39388,7 +39407,7 @@
       <c r="E41" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="F41" s="7">
+      <c r="F41" s="39">
         <v>24570</v>
       </c>
       <c r="G41" s="2" t="s">
@@ -39464,7 +39483,7 @@
       <c r="E42" s="2" t="s">
         <v>1546</v>
       </c>
-      <c r="F42" s="7">
+      <c r="F42" s="39">
         <v>26090</v>
       </c>
       <c r="G42" s="2" t="s">
@@ -39530,7 +39549,7 @@
       <c r="E43" s="2" t="s">
         <v>992</v>
       </c>
-      <c r="F43" s="7">
+      <c r="F43" s="39">
         <v>26755</v>
       </c>
       <c r="G43" s="2" t="s">
@@ -39606,7 +39625,7 @@
       <c r="E44" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="F44" s="7">
+      <c r="F44" s="39">
         <v>25874</v>
       </c>
       <c r="G44" s="2" t="s">
@@ -39682,7 +39701,7 @@
       <c r="E45" s="2" t="s">
         <v>1553</v>
       </c>
-      <c r="F45" s="7">
+      <c r="F45" s="39">
         <v>25902</v>
       </c>
       <c r="G45" s="2" t="s">
@@ -39748,7 +39767,7 @@
       <c r="E46" s="2" t="s">
         <v>1100</v>
       </c>
-      <c r="F46" s="7">
+      <c r="F46" s="39">
         <v>22585</v>
       </c>
       <c r="G46" s="2" t="s">
@@ -39814,7 +39833,7 @@
       <c r="E47" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F47" s="7">
+      <c r="F47" s="39">
         <v>26443</v>
       </c>
       <c r="G47" s="2" t="s">
@@ -39880,7 +39899,7 @@
       <c r="E48" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F48" s="7">
+      <c r="F48" s="39">
         <v>25391</v>
       </c>
       <c r="G48" s="2" t="s">
@@ -39956,7 +39975,7 @@
       <c r="E49" s="2" t="s">
         <v>1323</v>
       </c>
-      <c r="F49" s="7">
+      <c r="F49" s="39">
         <v>25273</v>
       </c>
       <c r="G49" s="2" t="s">
@@ -40032,7 +40051,7 @@
       <c r="E50" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F50" s="7">
+      <c r="F50" s="39">
         <v>27465</v>
       </c>
       <c r="G50" s="2" t="s">
@@ -40108,7 +40127,7 @@
       <c r="E51" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F51" s="7">
+      <c r="F51" s="39">
         <v>26229</v>
       </c>
       <c r="G51" s="2" t="s">
@@ -40176,7 +40195,7 @@
       <c r="E52" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F52" s="7">
+      <c r="F52" s="39">
         <v>25487</v>
       </c>
       <c r="G52" s="2" t="s">
@@ -40252,7 +40271,7 @@
       <c r="E53" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="F53" s="7">
+      <c r="F53" s="39">
         <v>24743</v>
       </c>
       <c r="G53" s="2" t="s">
@@ -40328,7 +40347,7 @@
       <c r="E54" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F54" s="7">
+      <c r="F54" s="39">
         <v>26251</v>
       </c>
       <c r="G54" s="2" t="s">
@@ -40404,7 +40423,7 @@
       <c r="E55" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F55" s="7">
+      <c r="F55" s="39">
         <v>27093</v>
       </c>
       <c r="G55" s="2" t="s">
@@ -40480,7 +40499,7 @@
       <c r="E56" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F56" s="7">
+      <c r="F56" s="39">
         <v>26727</v>
       </c>
       <c r="G56" s="2" t="s">
@@ -40546,7 +40565,7 @@
       <c r="E57" s="2" t="s">
         <v>886</v>
       </c>
-      <c r="F57" s="7">
+      <c r="F57" s="39">
         <v>25885</v>
       </c>
       <c r="G57" s="2" t="s">
@@ -40612,7 +40631,7 @@
       <c r="E58" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F58" s="7">
+      <c r="F58" s="39">
         <v>26185</v>
       </c>
       <c r="G58" s="2" t="s">
@@ -40688,7 +40707,7 @@
       <c r="E59" s="2" t="s">
         <v>1616</v>
       </c>
-      <c r="F59" s="7">
+      <c r="F59" s="39">
         <v>25778</v>
       </c>
       <c r="G59" s="2" t="s">
@@ -40754,7 +40773,7 @@
       <c r="E60" s="2" t="s">
         <v>1597</v>
       </c>
-      <c r="F60" s="7">
+      <c r="F60" s="39">
         <v>25593</v>
       </c>
       <c r="G60" s="2" t="s">
@@ -40820,7 +40839,7 @@
       <c r="E61" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="F61" s="7">
+      <c r="F61" s="39">
         <v>25028</v>
       </c>
       <c r="G61" s="2" t="s">
@@ -40896,7 +40915,7 @@
       <c r="E62" s="2" t="s">
         <v>1623</v>
       </c>
-      <c r="F62" s="7">
+      <c r="F62" s="39">
         <v>26675</v>
       </c>
       <c r="G62" s="2" t="s">
@@ -40962,7 +40981,7 @@
       <c r="E63" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="F63" s="7">
+      <c r="F63" s="39">
         <v>25948</v>
       </c>
       <c r="G63" s="2" t="s">
@@ -41038,7 +41057,7 @@
       <c r="E64" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F64" s="7">
+      <c r="F64" s="39">
         <v>28279</v>
       </c>
       <c r="G64" s="2" t="s">
@@ -41104,7 +41123,7 @@
       <c r="E65" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F65" s="7">
+      <c r="F65" s="39">
         <v>28031</v>
       </c>
       <c r="G65" s="2" t="s">
@@ -41180,7 +41199,7 @@
       <c r="E66" s="2" t="s">
         <v>886</v>
       </c>
-      <c r="F66" s="7">
+      <c r="F66" s="39">
         <v>28005</v>
       </c>
       <c r="G66" s="2" t="s">
@@ -41246,7 +41265,7 @@
       <c r="E67" s="2" t="s">
         <v>1597</v>
       </c>
-      <c r="F67" s="7">
+      <c r="F67" s="39">
         <v>26600</v>
       </c>
       <c r="G67" s="2" t="s">
@@ -41312,7 +41331,7 @@
       <c r="E68" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F68" s="7">
+      <c r="F68" s="39">
         <v>26412</v>
       </c>
       <c r="G68" s="2" t="s">
@@ -41378,7 +41397,7 @@
       <c r="E69" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F69" s="7">
+      <c r="F69" s="39">
         <v>26111</v>
       </c>
       <c r="G69" s="2" t="s">
@@ -41444,7 +41463,7 @@
       <c r="E70" s="2" t="s">
         <v>1100</v>
       </c>
-      <c r="F70" s="7">
+      <c r="F70" s="39">
         <v>26439</v>
       </c>
       <c r="G70" s="2" t="s">
@@ -41508,7 +41527,7 @@
       <c r="E71" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F71" s="7">
+      <c r="F71" s="39">
         <v>26100</v>
       </c>
       <c r="G71" s="2" t="s">
@@ -41584,7 +41603,7 @@
       <c r="E72" s="2" t="s">
         <v>672</v>
       </c>
-      <c r="F72" s="7">
+      <c r="F72" s="39">
         <v>27252</v>
       </c>
       <c r="G72" s="2" t="s">
@@ -41650,7 +41669,7 @@
       <c r="E73" s="2" t="s">
         <v>1100</v>
       </c>
-      <c r="F73" s="7">
+      <c r="F73" s="39">
         <v>27879</v>
       </c>
       <c r="G73" s="2" t="s">
@@ -41714,7 +41733,7 @@
       <c r="E74" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="F74" s="7">
+      <c r="F74" s="39">
         <v>26912</v>
       </c>
       <c r="G74" s="2" t="s">
@@ -41790,7 +41809,7 @@
       <c r="E75" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F75" s="7">
+      <c r="F75" s="39">
         <v>27949</v>
       </c>
       <c r="G75" s="2" t="s">
@@ -41856,7 +41875,7 @@
       <c r="E76" s="2" t="s">
         <v>1323</v>
       </c>
-      <c r="F76" s="7">
+      <c r="F76" s="39">
         <v>26072</v>
       </c>
       <c r="G76" s="2" t="s">
@@ -41922,7 +41941,7 @@
       <c r="E77" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="F77" s="7">
+      <c r="F77" s="39">
         <v>26386</v>
       </c>
       <c r="G77" s="2" t="s">
@@ -41990,7 +42009,7 @@
       <c r="E78" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F78" s="7">
+      <c r="F78" s="39">
         <v>27535</v>
       </c>
       <c r="G78" s="2" t="s">
@@ -42066,7 +42085,7 @@
       <c r="E79" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F79" s="7">
+      <c r="F79" s="39">
         <v>26567</v>
       </c>
       <c r="G79" s="2" t="s">
@@ -42132,7 +42151,7 @@
       <c r="E80" s="2" t="s">
         <v>1703</v>
       </c>
-      <c r="F80" s="7">
+      <c r="F80" s="39">
         <v>26403</v>
       </c>
       <c r="G80" s="2" t="s">
@@ -42198,7 +42217,7 @@
       <c r="E81" s="2" t="s">
         <v>1729</v>
       </c>
-      <c r="F81" s="7">
+      <c r="F81" s="39">
         <v>27287</v>
       </c>
       <c r="G81" s="2" t="s">
@@ -42264,7 +42283,7 @@
       <c r="E82" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="F82" s="7">
+      <c r="F82" s="39">
         <v>27833</v>
       </c>
       <c r="G82" s="2" t="s">
@@ -42330,7 +42349,7 @@
       <c r="E83" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="F83" s="7">
+      <c r="F83" s="39">
         <v>28135</v>
       </c>
       <c r="G83" s="2" t="s">
@@ -42404,7 +42423,7 @@
       <c r="E84" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="F84" s="7">
+      <c r="F84" s="39">
         <v>29089</v>
       </c>
       <c r="G84" s="2" t="s">
@@ -42470,7 +42489,7 @@
       <c r="E85" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F85" s="7">
+      <c r="F85" s="39">
         <v>29981</v>
       </c>
       <c r="G85" s="2" t="s">
@@ -42544,7 +42563,7 @@
       <c r="E86" s="2" t="s">
         <v>1743</v>
       </c>
-      <c r="F86" s="7">
+      <c r="F86" s="39">
         <v>29179</v>
       </c>
       <c r="G86" s="2" t="s">
@@ -42610,7 +42629,7 @@
       <c r="E87" s="2" t="s">
         <v>1763</v>
       </c>
-      <c r="F87" s="7">
+      <c r="F87" s="39">
         <v>28186</v>
       </c>
       <c r="G87" s="2" t="s">
@@ -42676,7 +42695,7 @@
       <c r="E88" s="2" t="s">
         <v>1750</v>
       </c>
-      <c r="F88" s="7">
+      <c r="F88" s="39">
         <v>29355</v>
       </c>
       <c r="G88" s="2" t="s">
@@ -42742,7 +42761,7 @@
       <c r="E89" s="2" t="s">
         <v>1736</v>
       </c>
-      <c r="F89" s="7">
+      <c r="F89" s="39">
         <v>29114</v>
       </c>
       <c r="G89" s="2" t="s">
@@ -42808,7 +42827,7 @@
       <c r="E90" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="F90" s="7">
+      <c r="F90" s="39">
         <v>29579</v>
       </c>
       <c r="G90" s="2" t="s">
@@ -42874,7 +42893,7 @@
       <c r="E91" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F91" s="7">
+      <c r="F91" s="39">
         <v>29367</v>
       </c>
       <c r="G91" s="2" t="s">
@@ -42940,7 +42959,7 @@
       <c r="E92" s="2" t="s">
         <v>1795</v>
       </c>
-      <c r="F92" s="7">
+      <c r="F92" s="39">
         <v>29335</v>
       </c>
       <c r="G92" s="2" t="s">
@@ -43006,7 +43025,7 @@
       <c r="E93" s="2" t="s">
         <v>1788</v>
       </c>
-      <c r="F93" s="7">
+      <c r="F93" s="39">
         <v>28626</v>
       </c>
       <c r="G93" s="2" t="s">
@@ -43072,7 +43091,7 @@
       <c r="E94" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F94" s="7">
+      <c r="F94" s="39">
         <v>31517</v>
       </c>
       <c r="G94" s="2" t="s">
@@ -43138,7 +43157,7 @@
       <c r="E95" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="F95" s="7">
+      <c r="F95" s="39">
         <v>25739</v>
       </c>
       <c r="G95" s="2" t="s">
@@ -43212,7 +43231,7 @@
       <c r="E96" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F96" s="7">
+      <c r="F96" s="39">
         <v>28236</v>
       </c>
       <c r="G96" s="2" t="s">
@@ -43278,7 +43297,7 @@
       <c r="E97" s="2" t="s">
         <v>483</v>
       </c>
-      <c r="F97" s="7">
+      <c r="F97" s="39">
         <v>30997</v>
       </c>
       <c r="G97" s="2" t="s">
@@ -43344,7 +43363,7 @@
       <c r="E98" s="2" t="s">
         <v>1381</v>
       </c>
-      <c r="F98" s="7">
+      <c r="F98" s="39">
         <v>30840</v>
       </c>
       <c r="G98" s="2" t="s">
@@ -43410,7 +43429,7 @@
       <c r="E99" s="2" t="s">
         <v>1100</v>
       </c>
-      <c r="F99" s="7">
+      <c r="F99" s="39">
         <v>30646</v>
       </c>
       <c r="G99" s="2" t="s">
@@ -43474,7 +43493,7 @@
       <c r="E100" s="2" t="s">
         <v>1584</v>
       </c>
-      <c r="F100" s="7">
+      <c r="F100" s="39">
         <v>30634</v>
       </c>
       <c r="G100" s="2" t="s">
@@ -43540,7 +43559,7 @@
       <c r="E101" s="2" t="s">
         <v>1908</v>
       </c>
-      <c r="F101" s="7">
+      <c r="F101" s="39">
         <v>31829</v>
       </c>
       <c r="G101" s="2" t="s">
@@ -43606,7 +43625,7 @@
       <c r="E102" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F102" s="7">
+      <c r="F102" s="39">
         <v>30077</v>
       </c>
       <c r="G102" s="2" t="s">
@@ -43672,7 +43691,7 @@
       <c r="E103" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F103" s="7">
+      <c r="F103" s="39">
         <v>30492</v>
       </c>
       <c r="G103" s="2" t="s">
@@ -43738,7 +43757,7 @@
       <c r="E104" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F104" s="7">
+      <c r="F104" s="39">
         <v>30054</v>
       </c>
       <c r="G104" s="2" t="s">
@@ -43804,7 +43823,7 @@
       <c r="E105" s="2" t="s">
         <v>468</v>
       </c>
-      <c r="F105" s="7">
+      <c r="F105" s="39">
         <v>28910</v>
       </c>
       <c r="G105" s="2" t="s">
@@ -43870,7 +43889,7 @@
       <c r="E106" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="F106" s="7">
+      <c r="F106" s="39">
         <v>30116</v>
       </c>
       <c r="G106" s="2" t="s">
@@ -43946,7 +43965,7 @@
       <c r="E107" s="2" t="s">
         <v>1808</v>
       </c>
-      <c r="F107" s="7">
+      <c r="F107" s="39">
         <v>30177</v>
       </c>
       <c r="G107" s="2" t="s">
@@ -44012,7 +44031,7 @@
       <c r="E108" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F108" s="7">
+      <c r="F108" s="39">
         <v>29657</v>
       </c>
       <c r="G108" s="2" t="s">
@@ -44088,7 +44107,7 @@
       <c r="E109" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F109" s="7">
+      <c r="F109" s="39">
         <v>29943</v>
       </c>
       <c r="G109" s="2" t="s">
@@ -44154,7 +44173,7 @@
       <c r="E110" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="F110" s="7">
+      <c r="F110" s="39">
         <v>30026</v>
       </c>
       <c r="G110" s="2" t="s">
@@ -44230,7 +44249,7 @@
       <c r="E111" s="2" t="s">
         <v>1252</v>
       </c>
-      <c r="F111" s="7">
+      <c r="F111" s="39">
         <v>30537</v>
       </c>
       <c r="G111" s="2" t="s">
@@ -44298,7 +44317,7 @@
       <c r="E112" s="2" t="s">
         <v>1041</v>
       </c>
-      <c r="F112" s="7">
+      <c r="F112" s="39">
         <v>27910</v>
       </c>
       <c r="G112" s="2" t="s">
@@ -44364,7 +44383,7 @@
       <c r="E113" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F113" s="7">
+      <c r="F113" s="39">
         <v>28741</v>
       </c>
       <c r="G113" s="2" t="s">
@@ -44430,7 +44449,7 @@
       <c r="E114" s="2" t="s">
         <v>520</v>
       </c>
-      <c r="F114" s="7">
+      <c r="F114" s="39">
         <v>29001</v>
       </c>
       <c r="G114" s="2" t="s">
@@ -44496,7 +44515,7 @@
       <c r="E115" s="2" t="s">
         <v>1827</v>
       </c>
-      <c r="F115" s="7">
+      <c r="F115" s="39">
         <v>29558</v>
       </c>
       <c r="G115" s="2" t="s">
@@ -44562,7 +44581,7 @@
       <c r="E116" s="2" t="s">
         <v>1901</v>
       </c>
-      <c r="F116" s="7">
+      <c r="F116" s="39">
         <v>30464</v>
       </c>
       <c r="G116" s="2" t="s">
@@ -44628,7 +44647,7 @@
       <c r="E117" s="2" t="s">
         <v>872</v>
       </c>
-      <c r="F117" s="7">
+      <c r="F117" s="39">
         <v>29047</v>
       </c>
       <c r="G117" s="2" t="s">
@@ -44694,7 +44713,7 @@
       <c r="E118" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="F118" s="7">
+      <c r="F118" s="39">
         <v>29386</v>
       </c>
       <c r="G118" s="2" t="s">
@@ -44760,7 +44779,7 @@
       <c r="E119" s="2" t="s">
         <v>1597</v>
       </c>
-      <c r="F119" s="7">
+      <c r="F119" s="39">
         <v>28710</v>
       </c>
       <c r="G119" s="2" t="s">
@@ -44826,7 +44845,7 @@
       <c r="E120" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="F120" s="7">
+      <c r="F120" s="39">
         <v>29263</v>
       </c>
       <c r="G120" s="2" t="s">
@@ -44892,7 +44911,7 @@
       <c r="E121" s="2" t="s">
         <v>1864</v>
       </c>
-      <c r="F121" s="7">
+      <c r="F121" s="39">
         <v>28571</v>
       </c>
       <c r="G121" s="2" t="s">
@@ -44958,7 +44977,7 @@
       <c r="E122" s="2" t="s">
         <v>1003</v>
       </c>
-      <c r="F122" s="7">
+      <c r="F122" s="39">
         <v>28517</v>
       </c>
       <c r="G122" s="2" t="s">
@@ -45032,7 +45051,7 @@
       <c r="E123" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F123" s="7">
+      <c r="F123" s="39">
         <v>28738</v>
       </c>
       <c r="G123" s="2" t="s">
@@ -45106,7 +45125,7 @@
       <c r="E124" s="2" t="s">
         <v>1106</v>
       </c>
-      <c r="F124" s="7">
+      <c r="F124" s="39">
         <v>24810</v>
       </c>
       <c r="G124" s="2" t="s">
@@ -45180,7 +45199,7 @@
       <c r="E125" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F125" s="7">
+      <c r="F125" s="39">
         <v>30413</v>
       </c>
       <c r="G125" s="2" t="s">
@@ -45254,7 +45273,7 @@
       <c r="E126" s="2" t="s">
         <v>672</v>
       </c>
-      <c r="F126" s="7">
+      <c r="F126" s="39">
         <v>28648</v>
       </c>
       <c r="G126" s="2" t="s">
@@ -45320,7 +45339,7 @@
       <c r="E127" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="F127" s="7">
+      <c r="F127" s="39">
         <v>30720</v>
       </c>
       <c r="G127" s="2" t="s">
@@ -45386,7 +45405,7 @@
       <c r="E128" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F128" s="7">
+      <c r="F128" s="39">
         <v>30456</v>
       </c>
       <c r="G128" s="2" t="s">
@@ -45452,7 +45471,7 @@
       <c r="E129" s="2" t="s">
         <v>1939</v>
       </c>
-      <c r="F129" s="7">
+      <c r="F129" s="39">
         <v>27663</v>
       </c>
       <c r="G129" s="2" t="s">
@@ -45518,7 +45537,7 @@
       <c r="E130" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F130" s="7">
+      <c r="F130" s="39">
         <v>29526</v>
       </c>
       <c r="G130" s="2" t="s">
@@ -45584,7 +45603,7 @@
       <c r="E131" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F131" s="7">
+      <c r="F131" s="39">
         <v>29318</v>
       </c>
       <c r="G131" s="2" t="s">
@@ -45660,7 +45679,7 @@
       <c r="E132" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F132" s="7">
+      <c r="F132" s="39">
         <v>30628</v>
       </c>
       <c r="G132" s="2" t="s">
@@ -45736,7 +45755,7 @@
       <c r="E133" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="F133" s="7">
+      <c r="F133" s="39">
         <v>29522</v>
       </c>
       <c r="G133" s="2" t="s">
@@ -45812,7 +45831,7 @@
       <c r="E134" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F134" s="7">
+      <c r="F134" s="39">
         <v>29637</v>
       </c>
       <c r="G134" s="2" t="s">
@@ -45878,7 +45897,7 @@
       <c r="E135" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="F135" s="7">
+      <c r="F135" s="39">
         <v>28895</v>
       </c>
       <c r="G135" s="2" t="s">
@@ -45954,7 +45973,7 @@
       <c r="E136" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F136" s="7">
+      <c r="F136" s="39">
         <v>30617</v>
       </c>
       <c r="G136" s="20" t="s">
@@ -46030,7 +46049,7 @@
       <c r="E137" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F137" s="7">
+      <c r="F137" s="39">
         <v>30546</v>
       </c>
       <c r="G137" s="2" t="s">
@@ -46096,7 +46115,7 @@
       <c r="E138" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="F138" s="7">
+      <c r="F138" s="39">
         <v>30262</v>
       </c>
       <c r="G138" s="2" t="s">
@@ -46172,7 +46191,7 @@
       <c r="E139" s="2" t="s">
         <v>468</v>
       </c>
-      <c r="F139" s="7">
+      <c r="F139" s="39">
         <v>30609</v>
       </c>
       <c r="G139" s="2" t="s">
@@ -46238,7 +46257,7 @@
       <c r="E140" s="2" t="s">
         <v>941</v>
       </c>
-      <c r="F140" s="7">
+      <c r="F140" s="39">
         <v>29866</v>
       </c>
       <c r="G140" s="2" t="s">
@@ -46314,7 +46333,7 @@
       <c r="E141" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F141" s="7">
+      <c r="F141" s="39">
         <v>29354</v>
       </c>
       <c r="G141" s="2" t="s">
@@ -46390,7 +46409,7 @@
       <c r="E142" s="2" t="s">
         <v>468</v>
       </c>
-      <c r="F142" s="7">
+      <c r="F142" s="39">
         <v>30994</v>
       </c>
       <c r="G142" s="2" t="s">
@@ -46456,7 +46475,7 @@
       <c r="E143" s="2" t="s">
         <v>2027</v>
       </c>
-      <c r="F143" s="7">
+      <c r="F143" s="39">
         <v>30098</v>
       </c>
       <c r="G143" s="2" t="s">
@@ -46522,7 +46541,7 @@
       <c r="E144" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="F144" s="7">
+      <c r="F144" s="39">
         <v>31124</v>
       </c>
       <c r="G144" s="2" t="s">
@@ -46588,7 +46607,7 @@
       <c r="E145" s="2" t="s">
         <v>468</v>
       </c>
-      <c r="F145" s="7">
+      <c r="F145" s="39">
         <v>29818</v>
       </c>
       <c r="G145" s="2" t="s">
@@ -46654,7 +46673,7 @@
       <c r="E146" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="F146" s="7">
+      <c r="F146" s="39">
         <v>30770</v>
       </c>
       <c r="G146" s="2" t="s">
@@ -46730,7 +46749,7 @@
       <c r="E147" s="2" t="s">
         <v>1952</v>
       </c>
-      <c r="F147" s="7">
+      <c r="F147" s="39">
         <v>30251</v>
       </c>
       <c r="G147" s="2" t="s">
@@ -46796,7 +46815,7 @@
       <c r="E148" s="2" t="s">
         <v>468</v>
       </c>
-      <c r="F148" s="7">
+      <c r="F148" s="39">
         <v>28245</v>
       </c>
       <c r="G148" s="2" t="s">
@@ -46862,7 +46881,7 @@
       <c r="E149" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F149" s="7">
+      <c r="F149" s="39">
         <v>30150</v>
       </c>
       <c r="G149" s="2" t="s">
@@ -46928,7 +46947,7 @@
       <c r="E150" s="2" t="s">
         <v>1041</v>
       </c>
-      <c r="F150" s="7">
+      <c r="F150" s="39">
         <v>29307</v>
       </c>
       <c r="G150" s="2" t="s">
@@ -46994,7 +47013,7 @@
       <c r="E151" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="F151" s="7">
+      <c r="F151" s="39">
         <v>30511</v>
       </c>
       <c r="G151" s="2" t="s">
@@ -47070,7 +47089,7 @@
       <c r="E152" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F152" s="7">
+      <c r="F152" s="39">
         <v>29268</v>
       </c>
       <c r="G152" s="2" t="s">
@@ -47136,7 +47155,7 @@
       <c r="E153" s="2" t="s">
         <v>483</v>
       </c>
-      <c r="F153" s="7">
+      <c r="F153" s="39">
         <v>30206</v>
       </c>
       <c r="G153" s="2" t="s">
@@ -47202,7 +47221,7 @@
       <c r="E154" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F154" s="7">
+      <c r="F154" s="39">
         <v>29065</v>
       </c>
       <c r="G154" s="2" t="s">
@@ -47268,7 +47287,7 @@
       <c r="E155" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="F155" s="7">
+      <c r="F155" s="39">
         <v>29320</v>
       </c>
       <c r="G155" s="2" t="s">
@@ -47334,7 +47353,7 @@
       <c r="E156" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="F156" s="7">
+      <c r="F156" s="39">
         <v>31397</v>
       </c>
       <c r="G156" s="2" t="s">
@@ -47410,7 +47429,7 @@
       <c r="E157" s="2" t="s">
         <v>2077</v>
       </c>
-      <c r="F157" s="7">
+      <c r="F157" s="39">
         <v>31366</v>
       </c>
       <c r="G157" s="2" t="s">
@@ -47476,7 +47495,7 @@
       <c r="E158" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="F158" s="7">
+      <c r="F158" s="39">
         <v>31620</v>
       </c>
       <c r="G158" s="2" t="s">
@@ -47552,7 +47571,7 @@
       <c r="E159" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F159" s="7">
+      <c r="F159" s="39">
         <v>30836</v>
       </c>
       <c r="G159" s="2" t="s">
@@ -47628,7 +47647,7 @@
       <c r="E160" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="F160" s="7">
+      <c r="F160" s="39">
         <v>30402</v>
       </c>
       <c r="G160" s="2" t="s">
@@ -47704,7 +47723,7 @@
       <c r="E161" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F161" s="7">
+      <c r="F161" s="39">
         <v>30746</v>
       </c>
       <c r="G161" s="2" t="s">
@@ -47780,7 +47799,7 @@
       <c r="E162" s="2" t="s">
         <v>1041</v>
       </c>
-      <c r="F162" s="7">
+      <c r="F162" s="39">
         <v>31308</v>
       </c>
       <c r="G162" s="2" t="s">
@@ -47856,7 +47875,7 @@
       <c r="E163" s="2" t="s">
         <v>1041</v>
       </c>
-      <c r="F163" s="7">
+      <c r="F163" s="39">
         <v>30142</v>
       </c>
       <c r="G163" s="2" t="s">
@@ -47922,7 +47941,7 @@
       <c r="E164" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F164" s="7">
+      <c r="F164" s="39">
         <v>31208</v>
       </c>
       <c r="G164" s="2" t="s">
@@ -47998,7 +48017,7 @@
       <c r="E165" s="2" t="s">
         <v>1323</v>
       </c>
-      <c r="F165" s="7">
+      <c r="F165" s="39">
         <v>31112</v>
       </c>
       <c r="G165" s="2" t="s">
@@ -48064,7 +48083,7 @@
       <c r="E166" s="2" t="s">
         <v>2070</v>
       </c>
-      <c r="F166" s="7">
+      <c r="F166" s="39">
         <v>29383</v>
       </c>
       <c r="G166" s="2" t="s">
@@ -48130,7 +48149,7 @@
       <c r="E167" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="F167" s="7">
+      <c r="F167" s="39">
         <v>30790</v>
       </c>
       <c r="G167" s="2" t="s">
@@ -48196,7 +48215,7 @@
       <c r="E168" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F168" s="7">
+      <c r="F168" s="39">
         <v>31594</v>
       </c>
       <c r="G168" s="2" t="s">
@@ -48262,7 +48281,7 @@
       <c r="E169" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F169" s="7">
+      <c r="F169" s="39">
         <v>29788</v>
       </c>
       <c r="G169" s="2" t="s">
@@ -48338,7 +48357,7 @@
       <c r="E170" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="F170" s="7">
+      <c r="F170" s="39">
         <v>30272</v>
       </c>
       <c r="G170" s="2" t="s">
@@ -48414,7 +48433,7 @@
       <c r="E171" s="2" t="s">
         <v>1184</v>
       </c>
-      <c r="F171" s="7">
+      <c r="F171" s="39">
         <v>30755</v>
       </c>
       <c r="G171" s="2" t="s">
@@ -48480,7 +48499,7 @@
       <c r="E172" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F172" s="7">
+      <c r="F172" s="39">
         <v>30118</v>
       </c>
       <c r="G172" s="2" t="s">
@@ -48546,7 +48565,7 @@
       <c r="E173" s="2" t="s">
         <v>536</v>
       </c>
-      <c r="F173" s="7">
+      <c r="F173" s="39">
         <v>31160</v>
       </c>
       <c r="G173" s="2" t="s">
@@ -48612,7 +48631,7 @@
       <c r="E174" s="2" t="s">
         <v>680</v>
       </c>
-      <c r="F174" s="7">
+      <c r="F174" s="39">
         <v>30975</v>
       </c>
       <c r="G174" s="20" t="s">
@@ -48688,7 +48707,7 @@
       <c r="E175" s="2" t="s">
         <v>1114</v>
       </c>
-      <c r="F175" s="7">
+      <c r="F175" s="39">
         <v>30650</v>
       </c>
       <c r="G175" s="2" t="s">
@@ -48762,7 +48781,7 @@
       <c r="E176" s="2" t="s">
         <v>1114</v>
       </c>
-      <c r="F176" s="7">
+      <c r="F176" s="39">
         <v>28975</v>
       </c>
       <c r="G176" s="2" t="s">
@@ -48836,7 +48855,7 @@
       <c r="E177" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="F177" s="7">
+      <c r="F177" s="39">
         <v>31728</v>
       </c>
       <c r="G177" s="2" t="s">
@@ -48902,7 +48921,7 @@
       <c r="E178" s="2" t="s">
         <v>1584</v>
       </c>
-      <c r="F178" s="7">
+      <c r="F178" s="39">
         <v>31528</v>
       </c>
       <c r="G178" s="2" t="s">
@@ -48968,7 +48987,7 @@
       <c r="E179" s="2" t="s">
         <v>2132</v>
       </c>
-      <c r="F179" s="7">
+      <c r="F179" s="39">
         <v>31783</v>
       </c>
       <c r="G179" s="2" t="s">
@@ -49034,7 +49053,7 @@
       <c r="E180" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F180" s="7">
+      <c r="F180" s="39">
         <v>31562</v>
       </c>
       <c r="G180" s="2" t="s">
@@ -49110,7 +49129,7 @@
       <c r="E181" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F181" s="7">
+      <c r="F181" s="39">
         <v>30909</v>
       </c>
       <c r="G181" s="2" t="s">
@@ -49174,7 +49193,7 @@
       <c r="E182" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="F182" s="7">
+      <c r="F182" s="39">
         <v>31994</v>
       </c>
       <c r="G182" s="2" t="s">
@@ -49240,7 +49259,7 @@
       <c r="E183" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F183" s="7">
+      <c r="F183" s="39">
         <v>31414</v>
       </c>
       <c r="G183" s="2" t="s">
@@ -49316,7 +49335,7 @@
       <c r="E184" s="2" t="s">
         <v>1057</v>
       </c>
-      <c r="F184" s="7">
+      <c r="F184" s="39">
         <v>31753</v>
       </c>
       <c r="G184" s="2" t="s">
@@ -49392,7 +49411,7 @@
       <c r="E185" s="2" t="s">
         <v>1252</v>
       </c>
-      <c r="F185" s="7">
+      <c r="F185" s="39">
         <v>30658</v>
       </c>
       <c r="G185" s="2" t="s">
@@ -49458,7 +49477,7 @@
       <c r="E186" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="F186" s="7">
+      <c r="F186" s="39">
         <v>30565</v>
       </c>
       <c r="G186" s="2" t="s">
@@ -49524,7 +49543,7 @@
       <c r="E187" s="2" t="s">
         <v>1011</v>
       </c>
-      <c r="F187" s="7">
+      <c r="F187" s="39">
         <v>29586</v>
       </c>
       <c r="G187" s="2" t="s">
@@ -49598,7 +49617,7 @@
       <c r="E188" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F188" s="7">
+      <c r="F188" s="39">
         <v>30751</v>
       </c>
       <c r="G188" s="2" t="s">
@@ -49664,7 +49683,7 @@
       <c r="E189" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F189" s="7">
+      <c r="F189" s="39">
         <v>30330</v>
       </c>
       <c r="G189" s="2" t="s">
@@ -49730,7 +49749,7 @@
       <c r="E190" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="F190" s="7">
+      <c r="F190" s="39">
         <v>29592</v>
       </c>
       <c r="G190" s="2" t="s">
@@ -49796,7 +49815,7 @@
       <c r="E191" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F191" s="7">
+      <c r="F191" s="39">
         <v>31177</v>
       </c>
       <c r="G191" s="2" t="s">
@@ -49872,7 +49891,7 @@
       <c r="E192" s="2" t="s">
         <v>1827</v>
       </c>
-      <c r="F192" s="7">
+      <c r="F192" s="39">
         <v>30204</v>
       </c>
       <c r="G192" s="2" t="s">
@@ -49938,7 +49957,7 @@
       <c r="E193" s="2" t="s">
         <v>2187</v>
       </c>
-      <c r="F193" s="7">
+      <c r="F193" s="39">
         <v>30550</v>
       </c>
       <c r="G193" s="2" t="s">
@@ -50004,7 +50023,7 @@
       <c r="E194" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="F194" s="7">
+      <c r="F194" s="39">
         <v>31017</v>
       </c>
       <c r="G194" s="2" t="s">
@@ -50070,7 +50089,7 @@
       <c r="E195" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F195" s="7">
+      <c r="F195" s="39">
         <v>31103</v>
       </c>
       <c r="G195" s="2" t="s">
@@ -50136,7 +50155,7 @@
       <c r="E196" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F196" s="7">
+      <c r="F196" s="39">
         <v>30076</v>
       </c>
       <c r="G196" s="2" t="s">
@@ -50202,7 +50221,7 @@
       <c r="E197" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F197" s="7">
+      <c r="F197" s="39">
         <v>31136</v>
       </c>
       <c r="G197" s="2" t="s">
@@ -50268,7 +50287,7 @@
       <c r="E198" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="F198" s="7">
+      <c r="F198" s="39">
         <v>31086</v>
       </c>
       <c r="G198" s="2" t="s">
@@ -50344,7 +50363,7 @@
       <c r="E199" s="2" t="s">
         <v>1129</v>
       </c>
-      <c r="F199" s="7">
+      <c r="F199" s="39">
         <v>29655</v>
       </c>
       <c r="G199" s="2" t="s">
@@ -50418,7 +50437,7 @@
       <c r="E200" s="2" t="s">
         <v>800</v>
       </c>
-      <c r="F200" s="7">
+      <c r="F200" s="39">
         <v>32407</v>
       </c>
       <c r="G200" s="2" t="s">
@@ -50484,7 +50503,7 @@
       <c r="E201" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="F201" s="7">
+      <c r="F201" s="39">
         <v>33364</v>
       </c>
       <c r="G201" s="2" t="s">
@@ -50558,7 +50577,7 @@
       <c r="E202" s="2" t="s">
         <v>1137</v>
       </c>
-      <c r="F202" s="7">
+      <c r="F202" s="39">
         <v>33165</v>
       </c>
       <c r="G202" s="2" t="s">
@@ -50632,7 +50651,7 @@
       <c r="E203" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="F203" s="7">
+      <c r="F203" s="39">
         <v>31917</v>
       </c>
       <c r="G203" s="2" t="s">
@@ -50698,7 +50717,7 @@
       <c r="E204" s="2" t="s">
         <v>2224</v>
       </c>
-      <c r="F204" s="7">
+      <c r="F204" s="39">
         <v>31040</v>
       </c>
       <c r="G204" s="2" t="s">
@@ -50764,7 +50783,7 @@
       <c r="E205" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F205" s="7">
+      <c r="F205" s="39">
         <v>30779</v>
       </c>
       <c r="G205" s="2" t="s">
@@ -50840,7 +50859,7 @@
       <c r="E206" s="2" t="s">
         <v>1252</v>
       </c>
-      <c r="F206" s="7">
+      <c r="F206" s="39">
         <v>29731</v>
       </c>
       <c r="G206" s="2" t="s">
@@ -50906,7 +50925,7 @@
       <c r="E207" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="F207" s="7">
+      <c r="F207" s="39">
         <v>30918</v>
       </c>
       <c r="G207" s="2" t="s">
@@ -50972,7 +50991,7 @@
       <c r="E208" s="2" t="s">
         <v>648</v>
       </c>
-      <c r="F208" s="7">
+      <c r="F208" s="39">
         <v>32509</v>
       </c>
       <c r="G208" s="2" t="s">
@@ -51038,7 +51057,7 @@
       <c r="E209" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F209" s="7">
+      <c r="F209" s="39">
         <v>32782</v>
       </c>
       <c r="G209" s="2" t="s">
@@ -51110,7 +51129,7 @@
       <c r="E210" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="F210" s="7">
+      <c r="F210" s="39">
         <v>29762</v>
       </c>
       <c r="G210" s="2" t="s">
@@ -51186,7 +51205,7 @@
       <c r="E211" s="2" t="s">
         <v>1100</v>
       </c>
-      <c r="F211" s="7">
+      <c r="F211" s="39">
         <v>32096</v>
       </c>
       <c r="G211" s="2" t="s">
@@ -51252,7 +51271,7 @@
       <c r="E212" s="2" t="s">
         <v>680</v>
       </c>
-      <c r="F212" s="7">
+      <c r="F212" s="39">
         <v>31823</v>
       </c>
       <c r="G212" s="2" t="s">
@@ -51328,7 +51347,7 @@
       <c r="E213" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="F213" s="7">
+      <c r="F213" s="39">
         <v>29924</v>
       </c>
       <c r="G213" s="2" t="s">
@@ -51404,7 +51423,7 @@
       <c r="E214" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F214" s="7">
+      <c r="F214" s="39">
         <v>31781</v>
       </c>
       <c r="G214" s="2" t="s">
@@ -51470,7 +51489,7 @@
       <c r="E215" s="2" t="s">
         <v>680</v>
       </c>
-      <c r="F215" s="7" t="s">
+      <c r="F215" s="39" t="s">
         <v>1081</v>
       </c>
       <c r="G215" s="20" t="s">
@@ -51539,7 +51558,7 @@
       <c r="E216" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F216" s="7">
+      <c r="F216" s="39">
         <v>32349</v>
       </c>
       <c r="G216" s="2" t="s">
@@ -51607,7 +51626,7 @@
       <c r="E217" s="2" t="s">
         <v>468</v>
       </c>
-      <c r="F217" s="7">
+      <c r="F217" s="39">
         <v>32396</v>
       </c>
       <c r="G217" s="2" t="s">
@@ -51683,7 +51702,7 @@
       <c r="E218" s="2" t="s">
         <v>2279</v>
       </c>
-      <c r="F218" s="7">
+      <c r="F218" s="39">
         <v>33041</v>
       </c>
       <c r="G218" s="2" t="s">
@@ -51749,7 +51768,7 @@
       <c r="E219" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="F219" s="7">
+      <c r="F219" s="39">
         <v>33176</v>
       </c>
       <c r="G219" s="2" t="s">
@@ -51823,7 +51842,7 @@
       <c r="E220" s="2" t="s">
         <v>1743</v>
       </c>
-      <c r="F220" s="7">
+      <c r="F220" s="39">
         <v>32190</v>
       </c>
       <c r="G220" s="2" t="s">
@@ -51889,7 +51908,7 @@
       <c r="E221" s="2" t="s">
         <v>2286</v>
       </c>
-      <c r="F221" s="7">
+      <c r="F221" s="39">
         <v>32330</v>
       </c>
       <c r="G221" s="2" t="s">
@@ -51955,7 +51974,7 @@
       <c r="E222" s="2" t="s">
         <v>1952</v>
       </c>
-      <c r="F222" s="7">
+      <c r="F222" s="39">
         <v>32820</v>
       </c>
       <c r="G222" s="2" t="s">
@@ -52021,7 +52040,7 @@
       <c r="E223" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F223" s="7">
+      <c r="F223" s="39">
         <v>32277</v>
       </c>
       <c r="G223" s="2" t="s">
@@ -52097,7 +52116,7 @@
       <c r="E224" s="2" t="s">
         <v>886</v>
       </c>
-      <c r="F224" s="7">
+      <c r="F224" s="39">
         <v>33411</v>
       </c>
       <c r="G224" s="2" t="s">
@@ -52163,7 +52182,7 @@
       <c r="E225" s="2" t="s">
         <v>2305</v>
       </c>
-      <c r="F225" s="7">
+      <c r="F225" s="39">
         <v>33381</v>
       </c>
       <c r="G225" s="2" t="s">
@@ -52229,7 +52248,7 @@
       <c r="E226" s="2" t="s">
         <v>2279</v>
       </c>
-      <c r="F226" s="7">
+      <c r="F226" s="39">
         <v>33044</v>
       </c>
       <c r="G226" s="2" t="s">
@@ -52295,7 +52314,7 @@
       <c r="E227" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F227" s="7">
+      <c r="F227" s="39">
         <v>33446</v>
       </c>
       <c r="G227" s="2" t="s">
@@ -52371,7 +52390,7 @@
       <c r="E228" s="2" t="s">
         <v>2318</v>
       </c>
-      <c r="F228" s="7">
+      <c r="F228" s="39">
         <v>33599</v>
       </c>
       <c r="G228" s="2" t="s">
@@ -52437,7 +52456,7 @@
       <c r="E229" s="2" t="s">
         <v>672</v>
       </c>
-      <c r="F229" s="7">
+      <c r="F229" s="39">
         <v>33365</v>
       </c>
       <c r="G229" s="2" t="s">
@@ -52503,7 +52522,7 @@
       <c r="E230" s="2" t="s">
         <v>2337</v>
       </c>
-      <c r="F230" s="7">
+      <c r="F230" s="39">
         <v>32238</v>
       </c>
       <c r="G230" s="2" t="s">
@@ -52569,7 +52588,7 @@
       <c r="E231" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="F231" s="7">
+      <c r="F231" s="39">
         <v>33147</v>
       </c>
       <c r="G231" s="2" t="s">
@@ -52635,7 +52654,7 @@
       <c r="E232" s="2" t="s">
         <v>1460</v>
       </c>
-      <c r="F232" s="7">
+      <c r="F232" s="39">
         <v>33431</v>
       </c>
       <c r="G232" s="2" t="s">
@@ -52701,7 +52720,7 @@
       <c r="E233" s="2" t="s">
         <v>672</v>
       </c>
-      <c r="F233" s="7">
+      <c r="F233" s="39">
         <v>33836</v>
       </c>
       <c r="G233" s="2" t="s">
@@ -52767,7 +52786,7 @@
       <c r="E234" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F234" s="7">
+      <c r="F234" s="39">
         <v>35108</v>
       </c>
       <c r="G234" s="2" t="s">
@@ -52841,7 +52860,7 @@
       <c r="E235" s="2" t="s">
         <v>498</v>
       </c>
-      <c r="F235" s="7">
+      <c r="F235" s="39">
         <v>34594</v>
       </c>
       <c r="G235" s="2" t="s">
@@ -52917,7 +52936,7 @@
       <c r="E236" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F236" s="7">
+      <c r="F236" s="39">
         <v>33962</v>
       </c>
       <c r="G236" s="2" t="s">
@@ -52993,7 +53012,7 @@
       <c r="E237" s="2" t="s">
         <v>483</v>
       </c>
-      <c r="F237" s="7">
+      <c r="F237" s="39">
         <v>33365</v>
       </c>
       <c r="G237" s="2" t="s">
@@ -53069,7 +53088,7 @@
       <c r="E238" s="2" t="s">
         <v>528</v>
       </c>
-      <c r="F238" s="7">
+      <c r="F238" s="39">
         <v>33931</v>
       </c>
       <c r="G238" s="2" t="s">
@@ -53145,7 +53164,7 @@
       <c r="E239" s="2" t="s">
         <v>561</v>
       </c>
-      <c r="F239" s="7">
+      <c r="F239" s="39">
         <v>34908</v>
       </c>
       <c r="G239" s="2" t="s">
@@ -53221,7 +53240,7 @@
       <c r="E240" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F240" s="7">
+      <c r="F240" s="39">
         <v>34510</v>
       </c>
       <c r="G240" s="2" t="s">
@@ -53297,7 +53316,7 @@
       <c r="E241" s="2" t="s">
         <v>536</v>
       </c>
-      <c r="F241" s="7">
+      <c r="F241" s="39">
         <v>34231</v>
       </c>
       <c r="G241" s="2" t="s">
@@ -53373,7 +53392,7 @@
       <c r="E242" s="2" t="s">
         <v>483</v>
       </c>
-      <c r="F242" s="7">
+      <c r="F242" s="39">
         <v>35360</v>
       </c>
       <c r="G242" s="2" t="s">
@@ -53449,7 +53468,7 @@
       <c r="E243" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="F243" s="7">
+      <c r="F243" s="39">
         <v>34626</v>
       </c>
       <c r="G243" s="2" t="s">
@@ -53525,7 +53544,7 @@
       <c r="E244" s="2" t="s">
         <v>512</v>
       </c>
-      <c r="F244" s="7">
+      <c r="F244" s="39">
         <v>33432</v>
       </c>
       <c r="G244" s="2" t="s">
@@ -53601,7 +53620,7 @@
       <c r="E245" s="2" t="s">
         <v>520</v>
       </c>
-      <c r="F245" s="7">
+      <c r="F245" s="39">
         <v>33882</v>
       </c>
       <c r="G245" s="2" t="s">
@@ -53677,7 +53696,7 @@
       <c r="E246" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="F246" s="7">
+      <c r="F246" s="39">
         <v>33061</v>
       </c>
       <c r="G246" s="2" t="s">
@@ -53753,7 +53772,7 @@
       <c r="E247" s="2" t="s">
         <v>1089</v>
       </c>
-      <c r="F247" s="7">
+      <c r="F247" s="39">
         <v>33913</v>
       </c>
       <c r="G247" s="2" t="s">
@@ -53829,7 +53848,7 @@
       <c r="E248" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="F248" s="7">
+      <c r="F248" s="39">
         <v>34976</v>
       </c>
       <c r="G248" s="20" t="s">
@@ -53905,7 +53924,7 @@
       <c r="E249" s="2" t="s">
         <v>648</v>
       </c>
-      <c r="F249" s="7">
+      <c r="F249" s="39">
         <v>35674</v>
       </c>
       <c r="G249" s="20" t="s">
@@ -53981,7 +54000,7 @@
       <c r="E250" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="F250" s="7">
+      <c r="F250" s="39">
         <v>33901</v>
       </c>
       <c r="G250" s="20" t="s">
@@ -54057,7 +54076,7 @@
       <c r="E251" s="2" t="s">
         <v>585</v>
       </c>
-      <c r="F251" s="7">
+      <c r="F251" s="39">
         <v>33705</v>
       </c>
       <c r="G251" s="20" t="s">
@@ -54133,7 +54152,7 @@
       <c r="E252" s="2" t="s">
         <v>617</v>
       </c>
-      <c r="F252" s="7">
+      <c r="F252" s="39">
         <v>34658</v>
       </c>
       <c r="G252" s="20" t="s">
@@ -54209,7 +54228,7 @@
       <c r="E253" s="3" t="s">
         <v>640</v>
       </c>
-      <c r="F253" s="26">
+      <c r="F253" s="40">
         <v>35271</v>
       </c>
       <c r="G253" s="3" t="s">
@@ -54285,7 +54304,7 @@
       <c r="E254" s="2" t="s">
         <v>625</v>
       </c>
-      <c r="F254" s="7">
+      <c r="F254" s="39">
         <v>34921</v>
       </c>
       <c r="G254" s="20" t="s">
@@ -54361,7 +54380,7 @@
       <c r="E255" s="2" t="s">
         <v>608</v>
       </c>
-      <c r="F255" s="7">
+      <c r="F255" s="39">
         <v>33951</v>
       </c>
       <c r="G255" s="20" t="s">
@@ -54437,7 +54456,7 @@
       <c r="E256" s="2" t="s">
         <v>594</v>
       </c>
-      <c r="F256" s="7">
+      <c r="F256" s="39">
         <v>33761</v>
       </c>
       <c r="G256" s="20" t="s">
@@ -54513,7 +54532,7 @@
       <c r="E257" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="F257" s="7">
+      <c r="F257" s="39">
         <v>35494</v>
       </c>
       <c r="G257" s="20" t="s">
@@ -54583,7 +54602,7 @@
       <c r="E258" s="2" t="s">
         <v>579</v>
       </c>
-      <c r="F258" s="7">
+      <c r="F258" s="39">
         <v>33673</v>
       </c>
       <c r="G258" s="20" t="s">
@@ -54659,7 +54678,7 @@
       <c r="E259" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="F259" s="7">
+      <c r="F259" s="39">
         <v>36900</v>
       </c>
       <c r="G259" s="2" t="s">
@@ -54733,7 +54752,7 @@
       <c r="E260" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F260" s="7">
+      <c r="F260" s="39">
         <v>35701</v>
       </c>
       <c r="G260" s="2" t="s">
@@ -54809,7 +54828,7 @@
       <c r="E261" s="2" t="s">
         <v>792</v>
       </c>
-      <c r="F261" s="7">
+      <c r="F261" s="39">
         <v>34924</v>
       </c>
       <c r="G261" s="2" t="s">
@@ -54885,7 +54904,7 @@
       <c r="E262" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F262" s="7">
+      <c r="F262" s="39">
         <v>33154</v>
       </c>
       <c r="G262" s="2" t="s">
@@ -54961,7 +54980,7 @@
       <c r="E263" s="2" t="s">
         <v>754</v>
       </c>
-      <c r="F263" s="7">
+      <c r="F263" s="39">
         <v>34331</v>
       </c>
       <c r="G263" s="2" t="s">
@@ -55037,7 +55056,7 @@
       <c r="E264" s="2" t="s">
         <v>664</v>
       </c>
-      <c r="F264" s="7">
+      <c r="F264" s="39">
         <v>31703</v>
       </c>
       <c r="G264" s="2" t="s">
@@ -55113,7 +55132,7 @@
       <c r="E265" s="2" t="s">
         <v>680</v>
       </c>
-      <c r="F265" s="7">
+      <c r="F265" s="39">
         <v>32029</v>
       </c>
       <c r="G265" s="2" t="s">
@@ -55189,7 +55208,7 @@
       <c r="E266" s="2" t="s">
         <v>838</v>
       </c>
-      <c r="F266" s="7">
+      <c r="F266" s="39">
         <v>35325</v>
       </c>
       <c r="G266" s="2" t="s">
@@ -55265,7 +55284,7 @@
       <c r="E267" s="2" t="s">
         <v>920</v>
       </c>
-      <c r="F267" s="7">
+      <c r="F267" s="39">
         <v>36065</v>
       </c>
       <c r="G267" s="2" t="s">
@@ -55341,7 +55360,7 @@
       <c r="E268" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F268" s="7">
+      <c r="F268" s="39">
         <v>34637</v>
       </c>
       <c r="G268" s="2" t="s">
@@ -55417,7 +55436,7 @@
       <c r="E269" s="2" t="s">
         <v>498</v>
       </c>
-      <c r="F269" s="7">
+      <c r="F269" s="39">
         <v>34790</v>
       </c>
       <c r="G269" s="2" t="s">
@@ -55493,7 +55512,7 @@
       <c r="E270" s="2" t="s">
         <v>863</v>
       </c>
-      <c r="F270" s="7">
+      <c r="F270" s="39">
         <v>35755</v>
       </c>
       <c r="G270" s="2" t="s">
@@ -55569,7 +55588,7 @@
       <c r="E271" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F271" s="7">
+      <c r="F271" s="39">
         <v>35974</v>
       </c>
       <c r="G271" s="2" t="s">
@@ -55645,7 +55664,7 @@
       <c r="E272" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F272" s="7">
+      <c r="F272" s="39">
         <v>35107</v>
       </c>
       <c r="G272" s="2" t="s">
@@ -55721,7 +55740,7 @@
       <c r="E273" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="F273" s="7">
+      <c r="F273" s="39">
         <v>36041</v>
       </c>
       <c r="G273" s="2" t="s">
@@ -55797,7 +55816,7 @@
       <c r="E274" s="2" t="s">
         <v>824</v>
       </c>
-      <c r="F274" s="7">
+      <c r="F274" s="39">
         <v>35257</v>
       </c>
       <c r="G274" s="2" t="s">
@@ -55873,7 +55892,7 @@
       <c r="E275" s="2" t="s">
         <v>800</v>
       </c>
-      <c r="F275" s="7">
+      <c r="F275" s="39">
         <v>35048</v>
       </c>
       <c r="G275" s="2" t="s">
@@ -55949,7 +55968,7 @@
       <c r="E276" s="2" t="s">
         <v>872</v>
       </c>
-      <c r="F276" s="7">
+      <c r="F276" s="39">
         <v>35758</v>
       </c>
       <c r="G276" s="2" t="s">
@@ -56025,7 +56044,7 @@
       <c r="E277" s="2" t="s">
         <v>680</v>
       </c>
-      <c r="F277" s="7">
+      <c r="F277" s="39">
         <v>35933</v>
       </c>
       <c r="G277" s="2" t="s">
@@ -56101,7 +56120,7 @@
       <c r="E278" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F278" s="7">
+      <c r="F278" s="39">
         <v>32458</v>
       </c>
       <c r="G278" s="2" t="s">
@@ -56177,7 +56196,7 @@
       <c r="E279" s="2" t="s">
         <v>717</v>
       </c>
-      <c r="F279" s="7">
+      <c r="F279" s="39">
         <v>33165</v>
       </c>
       <c r="G279" s="2" t="s">
@@ -56253,7 +56272,7 @@
       <c r="E280" s="2" t="s">
         <v>672</v>
       </c>
-      <c r="F280" s="7">
+      <c r="F280" s="39">
         <v>31726</v>
       </c>
       <c r="G280" s="2" t="s">
@@ -56329,7 +56348,7 @@
       <c r="E281" s="2" t="s">
         <v>880</v>
       </c>
-      <c r="F281" s="7">
+      <c r="F281" s="39">
         <v>35794</v>
       </c>
       <c r="G281" s="2" t="s">
@@ -56405,7 +56424,7 @@
       <c r="E282" s="2" t="s">
         <v>468</v>
       </c>
-      <c r="F282" s="7">
+      <c r="F282" s="39">
         <v>35436</v>
       </c>
       <c r="G282" s="2" t="s">
@@ -56481,7 +56500,7 @@
       <c r="E283" s="2" t="s">
         <v>688</v>
       </c>
-      <c r="F283" s="7">
+      <c r="F283" s="39">
         <v>32189</v>
       </c>
       <c r="G283" s="2" t="s">
@@ -56557,7 +56576,7 @@
       <c r="E284" s="2" t="s">
         <v>783</v>
       </c>
-      <c r="F284" s="7">
+      <c r="F284" s="39">
         <v>34815</v>
       </c>
       <c r="G284" s="2" t="s">
@@ -56633,7 +56652,7 @@
       <c r="E285" s="2" t="s">
         <v>672</v>
       </c>
-      <c r="F285" s="7">
+      <c r="F285" s="39">
         <v>35304</v>
       </c>
       <c r="G285" s="2" t="s">
@@ -56709,7 +56728,7 @@
       <c r="E286" s="2" t="s">
         <v>748</v>
       </c>
-      <c r="F286" s="7">
+      <c r="F286" s="39">
         <v>34050</v>
       </c>
       <c r="G286" s="2" t="s">
@@ -56785,7 +56804,7 @@
       <c r="E287" s="2" t="s">
         <v>702</v>
       </c>
-      <c r="F287" s="7">
+      <c r="F287" s="39">
         <v>32919</v>
       </c>
       <c r="G287" s="2" t="s">
@@ -56861,7 +56880,7 @@
       <c r="E288" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="F288" s="7">
+      <c r="F288" s="39">
         <v>35576</v>
       </c>
       <c r="G288" s="2" t="s">
@@ -56937,7 +56956,7 @@
       <c r="E289" s="2" t="s">
         <v>763</v>
       </c>
-      <c r="F289" s="7">
+      <c r="F289" s="39">
         <v>34625</v>
       </c>
       <c r="G289" s="2" t="s">
@@ -57013,7 +57032,7 @@
       <c r="E290" s="2" t="s">
         <v>816</v>
       </c>
-      <c r="F290" s="7">
+      <c r="F290" s="39">
         <v>35184</v>
       </c>
       <c r="G290" s="2" t="s">
@@ -57089,7 +57108,7 @@
       <c r="E291" s="2" t="s">
         <v>886</v>
       </c>
-      <c r="F291" s="7">
+      <c r="F291" s="39">
         <v>35798</v>
       </c>
       <c r="G291" s="2" t="s">
@@ -57165,7 +57184,7 @@
       <c r="E292" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="F292" s="7">
+      <c r="F292" s="39">
         <v>36356</v>
       </c>
       <c r="G292" s="2" t="s">
@@ -57241,7 +57260,7 @@
       <c r="E293" s="2" t="s">
         <v>731</v>
       </c>
-      <c r="F293" s="7">
+      <c r="F293" s="39">
         <v>33566</v>
       </c>
       <c r="G293" s="2" t="s">
@@ -57317,7 +57336,7 @@
       <c r="E294" s="2" t="s">
         <v>740</v>
       </c>
-      <c r="F294" s="7">
+      <c r="F294" s="39">
         <v>33584</v>
       </c>
       <c r="G294" s="2" t="s">
@@ -57393,7 +57412,7 @@
       <c r="E295" s="2" t="s">
         <v>792</v>
       </c>
-      <c r="F295" s="7">
+      <c r="F295" s="39">
         <v>35868</v>
       </c>
       <c r="G295" s="2" t="s">
@@ -57469,7 +57488,7 @@
       <c r="E296" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="F296" s="7">
+      <c r="F296" s="39">
         <v>33491</v>
       </c>
       <c r="G296" s="2" t="s">
@@ -57545,7 +57564,7 @@
       <c r="E297" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F297" s="7">
+      <c r="F297" s="39">
         <v>33499</v>
       </c>
       <c r="G297" s="2" t="s">
@@ -57619,7 +57638,7 @@
       <c r="E298" s="23" t="s">
         <v>280</v>
       </c>
-      <c r="F298" s="24">
+      <c r="F298" s="41">
         <v>35100</v>
       </c>
       <c r="G298" s="20" t="s">
@@ -57688,7 +57707,7 @@
       <c r="E299" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F299" s="7">
+      <c r="F299" s="39">
         <v>36475</v>
       </c>
       <c r="G299" s="2" t="s">
@@ -57762,7 +57781,7 @@
       <c r="E300" s="3" t="s">
         <v>2356</v>
       </c>
-      <c r="F300" s="26">
+      <c r="F300" s="40">
         <v>34797</v>
       </c>
       <c r="G300" s="3" t="s">
@@ -57828,7 +57847,7 @@
       <c r="E301" s="31" t="s">
         <v>432</v>
       </c>
-      <c r="F301" s="18">
+      <c r="F301" s="42">
         <v>28185</v>
       </c>
       <c r="G301" s="31" t="s">
@@ -57928,12 +57947,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="35e2c585-819f-4278-8a16-df2610a1755b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="a5904320-7c22-4772-b594-ceafc042e3d2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -58132,20 +58153,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="35e2c585-819f-4278-8a16-df2610a1755b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="a5904320-7c22-4772-b594-ceafc042e3d2" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{623689F7-DDC4-43DC-AB5C-EAB680CA80A6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5018FBA8-FFB9-4942-93FE-3D9DBCE7EB9C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="35e2c585-819f-4278-8a16-df2610a1755b"/>
+    <ds:schemaRef ds:uri="a5904320-7c22-4772-b594-ceafc042e3d2"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -58170,12 +58192,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5018FBA8-FFB9-4942-93FE-3D9DBCE7EB9C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{623689F7-DDC4-43DC-AB5C-EAB680CA80A6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="35e2c585-819f-4278-8a16-df2610a1755b"/>
-    <ds:schemaRef ds:uri="a5904320-7c22-4772-b594-ceafc042e3d2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>